<commit_message>
Lots of bug fixes and added some features
</commit_message>
<xml_diff>
--- a/Python/80518_Measurement Data_Lot XXX.xlsx
+++ b/Python/80518_Measurement Data_Lot XXX.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13512"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6828"/>
   </bookViews>
   <sheets>
     <sheet name="Lot_XXX" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -649,6 +648,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,7 +942,7 @@
   <dimension ref="B1:V290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,8 +950,7 @@
     <col min="1" max="1" width="11.44140625" style="2"/>
     <col min="2" max="2" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.44140625" style="2" customWidth="1"/>
-    <col min="6" max="10" width="9.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="10" width="9.44140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="9.44140625" style="38" customWidth="1"/>
@@ -966,133 +965,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="2"/>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="M2" s="2"/>
-      <c r="O2" s="16"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="M3" s="2"/>
-      <c r="O3" s="16"/>
-      <c r="Q3" s="16"/>
+      <c r="O3" s="15"/>
+      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="18">
         <v>136.69999999999999</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="2"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="16"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>80518</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="18">
         <v>30.175999999999998</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="2"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="16"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="20">
         <v>28</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="2"/>
-      <c r="Q6" s="16"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="D7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="I7" s="15"/>
       <c r="M7" s="2"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="O8" s="26" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="O8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="27" t="s">
+      <c r="P8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="Q8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="R8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="27"/>
-      <c r="T8" s="24"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
@@ -1107,74 +1106,74 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="O9" s="26" t="s">
+      <c r="O9" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="28" t="s">
+      <c r="P9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="28" t="s">
+      <c r="R9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="S9" s="28"/>
-      <c r="T9" s="29"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="28"/>
     </row>
     <row r="10" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="32" t="s">
+      <c r="O10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="33" t="s">
+      <c r="P10" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="33" t="s">
+      <c r="Q10" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="33" t="s">
+      <c r="R10" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="S10" s="33" t="s">
+      <c r="S10" s="32" t="s">
         <v>38</v>
       </c>
       <c r="T10" s="1"/>
@@ -1215,21 +1214,21 @@
         <v>28.315799999999999</v>
       </c>
       <c r="M11" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="33">
         <v>1.5788899999999999</v>
       </c>
-      <c r="Q11" s="34">
+      <c r="Q11" s="33">
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="R11" s="34">
+      <c r="R11" s="33">
         <v>-7.7999999999999999E-5</v>
       </c>
-      <c r="S11" s="35" t="s">
+      <c r="S11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T11" s="1"/>
@@ -1275,16 +1274,16 @@
       <c r="O12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="34">
+      <c r="P12" s="33">
         <v>1.57867</v>
       </c>
-      <c r="Q12" s="34">
+      <c r="Q12" s="33">
         <v>1.6699999999999999E-4</v>
       </c>
-      <c r="R12" s="34">
+      <c r="R12" s="33">
         <v>-5.3999999999999998E-5</v>
       </c>
-      <c r="S12" s="35" t="s">
+      <c r="S12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T12" s="1"/>
@@ -1330,16 +1329,16 @@
       <c r="O13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="34">
+      <c r="P13" s="33">
         <v>1.5694360000000001</v>
       </c>
-      <c r="Q13" s="34">
+      <c r="Q13" s="33">
         <v>5.8999999999999998E-5</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="33">
         <v>1.4200000000000001E-4</v>
       </c>
-      <c r="S13" s="35" t="s">
+      <c r="S13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T13" s="1"/>
@@ -1385,16 +1384,16 @@
       <c r="O14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P14" s="33">
         <v>1.568341</v>
       </c>
-      <c r="Q14" s="34">
+      <c r="Q14" s="33">
         <v>1.11E-4</v>
       </c>
-      <c r="R14" s="34">
+      <c r="R14" s="33">
         <v>2.6999999999999999E-5</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T14" s="1"/>
@@ -1440,16 +1439,16 @@
       <c r="O15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="33">
         <v>1.569852</v>
       </c>
-      <c r="Q15" s="34">
+      <c r="Q15" s="33">
         <v>-6.7999999999999999E-5</v>
       </c>
-      <c r="R15" s="34">
+      <c r="R15" s="33">
         <v>1E-4</v>
       </c>
-      <c r="S15" s="35" t="s">
+      <c r="S15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T15" s="1"/>
@@ -1495,16 +1494,16 @@
       <c r="O16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="33">
         <v>1.572408</v>
       </c>
-      <c r="Q16" s="34">
+      <c r="Q16" s="33">
         <v>1.1379999999999999E-3</v>
       </c>
-      <c r="R16" s="34">
+      <c r="R16" s="33">
         <v>9.2000000000000003E-4</v>
       </c>
-      <c r="S16" s="35" t="s">
+      <c r="S16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T16" s="1"/>
@@ -1550,16 +1549,16 @@
       <c r="O17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="34">
+      <c r="P17" s="33">
         <v>1.575404</v>
       </c>
-      <c r="Q17" s="34">
+      <c r="Q17" s="33">
         <v>1.1670000000000001E-3</v>
       </c>
-      <c r="R17" s="34">
+      <c r="R17" s="33">
         <v>9.2000000000000003E-4</v>
       </c>
-      <c r="S17" s="35" t="s">
+      <c r="S17" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T17" s="1"/>
@@ -1605,16 +1604,16 @@
       <c r="O18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="33">
         <v>1.5800380000000001</v>
       </c>
-      <c r="Q18" s="34">
+      <c r="Q18" s="33">
         <v>7.18E-4</v>
       </c>
-      <c r="R18" s="34">
+      <c r="R18" s="33">
         <v>5.2899999999999996E-4</v>
       </c>
-      <c r="S18" s="35" t="s">
+      <c r="S18" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T18" s="1"/>
@@ -1660,16 +1659,16 @@
       <c r="O19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="P19" s="34">
+      <c r="P19" s="33">
         <v>1.5820939999999999</v>
       </c>
-      <c r="Q19" s="34">
+      <c r="Q19" s="33">
         <v>1.2E-5</v>
       </c>
-      <c r="R19" s="34">
+      <c r="R19" s="33">
         <v>9.6000000000000002E-5</v>
       </c>
-      <c r="S19" s="35" t="s">
+      <c r="S19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T19" s="1"/>
@@ -1715,16 +1714,16 @@
       <c r="O20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="34">
+      <c r="P20" s="33">
         <v>1.5618890000000001</v>
       </c>
-      <c r="Q20" s="34">
+      <c r="Q20" s="33">
         <v>-3.8000000000000002E-5</v>
       </c>
-      <c r="R20" s="34">
+      <c r="R20" s="33">
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="S20" s="35" t="s">
+      <c r="S20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T20" s="1"/>
@@ -1770,16 +1769,16 @@
       <c r="O21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="P21" s="34">
+      <c r="P21" s="33">
         <v>1.561299</v>
       </c>
-      <c r="Q21" s="34">
+      <c r="Q21" s="33">
         <v>1.56E-4</v>
       </c>
-      <c r="R21" s="34">
+      <c r="R21" s="33">
         <v>-4.0000000000000003E-5</v>
       </c>
-      <c r="S21" s="35" t="s">
+      <c r="S21" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T21" s="1"/>
@@ -1825,16 +1824,16 @@
       <c r="O22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="34">
+      <c r="P22" s="33">
         <v>1.5755969999999999</v>
       </c>
-      <c r="Q22" s="34">
+      <c r="Q22" s="33">
         <v>1.25E-4</v>
       </c>
-      <c r="R22" s="34">
+      <c r="R22" s="33">
         <v>-4.5000000000000003E-5</v>
       </c>
-      <c r="S22" s="35" t="s">
+      <c r="S22" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T22" s="1"/>
@@ -1880,16 +1879,16 @@
       <c r="O23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="P23" s="34">
+      <c r="P23" s="33">
         <v>1.5767929999999999</v>
       </c>
-      <c r="Q23" s="34">
+      <c r="Q23" s="33">
         <v>1.1E-4</v>
       </c>
-      <c r="R23" s="34">
+      <c r="R23" s="33">
         <v>9.6000000000000002E-5</v>
       </c>
-      <c r="S23" s="35" t="s">
+      <c r="S23" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T23" s="1"/>
@@ -1935,16 +1934,16 @@
       <c r="O24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P24" s="34">
+      <c r="P24" s="33">
         <v>1.576632</v>
       </c>
-      <c r="Q24" s="34">
+      <c r="Q24" s="33">
         <v>2.52E-4</v>
       </c>
-      <c r="R24" s="34">
+      <c r="R24" s="33">
         <v>-4.3000000000000002E-5</v>
       </c>
-      <c r="S24" s="35" t="s">
+      <c r="S24" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T24" s="1"/>
@@ -1990,16 +1989,16 @@
       <c r="O25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="P25" s="34">
+      <c r="P25" s="33">
         <v>1.5768530000000001</v>
       </c>
-      <c r="Q25" s="34">
+      <c r="Q25" s="33">
         <v>4.6E-5</v>
       </c>
-      <c r="R25" s="34">
+      <c r="R25" s="33">
         <v>-8.7000000000000001E-5</v>
       </c>
-      <c r="S25" s="35" t="s">
+      <c r="S25" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T25" s="1"/>
@@ -2045,16 +2044,16 @@
       <c r="O26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="P26" s="34">
+      <c r="P26" s="33">
         <v>1.574605</v>
       </c>
-      <c r="Q26" s="34">
+      <c r="Q26" s="33">
         <v>-8.2999999999999998E-5</v>
       </c>
-      <c r="R26" s="34">
+      <c r="R26" s="33">
         <v>9.6000000000000002E-5</v>
       </c>
-      <c r="S26" s="35" t="s">
+      <c r="S26" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T26" s="1"/>
@@ -2100,16 +2099,16 @@
       <c r="O27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P27" s="34">
+      <c r="P27" s="33">
         <v>1.572308</v>
       </c>
-      <c r="Q27" s="34">
+      <c r="Q27" s="33">
         <v>2.9E-5</v>
       </c>
-      <c r="R27" s="34">
+      <c r="R27" s="33">
         <v>6.7999999999999999E-5</v>
       </c>
-      <c r="S27" s="35" t="s">
+      <c r="S27" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T27" s="1"/>
@@ -2155,16 +2154,16 @@
       <c r="O28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="P28" s="34">
+      <c r="P28" s="33">
         <v>1.5702579999999999</v>
       </c>
-      <c r="Q28" s="34">
+      <c r="Q28" s="33">
         <v>-2.8E-5</v>
       </c>
-      <c r="R28" s="34">
+      <c r="R28" s="33">
         <v>7.8999999999999996E-5</v>
       </c>
-      <c r="S28" s="35" t="s">
+      <c r="S28" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T28" s="1"/>
@@ -2210,16 +2209,16 @@
       <c r="O29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="P29" s="34">
+      <c r="P29" s="33">
         <v>1.5732409999999999</v>
       </c>
-      <c r="Q29" s="34">
+      <c r="Q29" s="33">
         <v>-2.5999999999999998E-5</v>
       </c>
-      <c r="R29" s="34">
+      <c r="R29" s="33">
         <v>-7.8999999999999996E-5</v>
       </c>
-      <c r="S29" s="35" t="s">
+      <c r="S29" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T29" s="1"/>
@@ -2265,16 +2264,16 @@
       <c r="O30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P30" s="34">
+      <c r="P30" s="33">
         <v>1.578055</v>
       </c>
-      <c r="Q30" s="34">
+      <c r="Q30" s="33">
         <v>-2.5000000000000001E-5</v>
       </c>
-      <c r="R30" s="34">
+      <c r="R30" s="33">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="S30" s="35" t="s">
+      <c r="S30" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T30" s="1"/>
@@ -2320,16 +2319,16 @@
       <c r="O31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="P31" s="34">
+      <c r="P31" s="33">
         <v>1.57694</v>
       </c>
-      <c r="Q31" s="34">
+      <c r="Q31" s="33">
         <v>-1.0000000000000001E-5</v>
       </c>
-      <c r="R31" s="34">
+      <c r="R31" s="33">
         <v>-6.6000000000000005E-5</v>
       </c>
-      <c r="S31" s="35" t="s">
+      <c r="S31" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T31" s="1"/>
@@ -2375,16 +2374,16 @@
       <c r="O32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P32" s="34">
+      <c r="P32" s="33">
         <v>1.5774239999999999</v>
       </c>
-      <c r="Q32" s="34">
+      <c r="Q32" s="33">
         <v>1.34E-4</v>
       </c>
-      <c r="R32" s="34">
+      <c r="R32" s="33">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="S32" s="35" t="s">
+      <c r="S32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T32" s="1"/>
@@ -2430,16 +2429,16 @@
       <c r="O33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P33" s="34">
+      <c r="P33" s="33">
         <v>1.573812</v>
       </c>
-      <c r="Q33" s="34">
+      <c r="Q33" s="33">
         <v>-9.0000000000000002E-6</v>
       </c>
-      <c r="R33" s="34">
+      <c r="R33" s="33">
         <v>7.8999999999999996E-5</v>
       </c>
-      <c r="S33" s="35" t="s">
+      <c r="S33" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T33" s="1"/>
@@ -2485,16 +2484,16 @@
       <c r="O34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P34" s="34">
+      <c r="P34" s="33">
         <v>1.576651</v>
       </c>
-      <c r="Q34" s="34">
+      <c r="Q34" s="33">
         <v>5.9699999999999998E-4</v>
       </c>
-      <c r="R34" s="34">
+      <c r="R34" s="33">
         <v>5.3600000000000002E-4</v>
       </c>
-      <c r="S34" s="35" t="s">
+      <c r="S34" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T34" s="1"/>
@@ -2540,16 +2539,16 @@
       <c r="O35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="P35" s="34">
+      <c r="P35" s="33">
         <v>1.569272</v>
       </c>
-      <c r="Q35" s="34">
+      <c r="Q35" s="33">
         <v>-2.5999999999999998E-5</v>
       </c>
-      <c r="R35" s="34">
+      <c r="R35" s="33">
         <v>5.1E-5</v>
       </c>
-      <c r="S35" s="35" t="s">
+      <c r="S35" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T35" s="1"/>
@@ -2595,16 +2594,16 @@
       <c r="O36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P36" s="34">
+      <c r="P36" s="33">
         <v>1.5648089999999999</v>
       </c>
-      <c r="Q36" s="34">
+      <c r="Q36" s="33">
         <v>1.16E-4</v>
       </c>
-      <c r="R36" s="34">
+      <c r="R36" s="33">
         <v>6.7999999999999999E-5</v>
       </c>
-      <c r="S36" s="35" t="s">
+      <c r="S36" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T36" s="1"/>
@@ -2650,16 +2649,16 @@
       <c r="O37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="P37" s="34">
+      <c r="P37" s="33">
         <v>1.5665439999999999</v>
       </c>
-      <c r="Q37" s="34">
+      <c r="Q37" s="33">
         <v>5.3000000000000001E-5</v>
       </c>
-      <c r="R37" s="34">
+      <c r="R37" s="33">
         <v>1.08E-4</v>
       </c>
-      <c r="S37" s="35" t="s">
+      <c r="S37" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T37" s="1"/>
@@ -2705,16 +2704,16 @@
       <c r="O38" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P38" s="34">
+      <c r="P38" s="33">
         <v>1.5695030000000001</v>
       </c>
-      <c r="Q38" s="34">
+      <c r="Q38" s="33">
         <v>-2.8E-5</v>
       </c>
-      <c r="R38" s="34">
+      <c r="R38" s="33">
         <v>1.25E-4</v>
       </c>
-      <c r="S38" s="35" t="s">
+      <c r="S38" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T38" s="1"/>
@@ -2760,16 +2759,16 @@
       <c r="O39" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="P39" s="34">
+      <c r="P39" s="33">
         <v>1.5683229999999999</v>
       </c>
-      <c r="Q39" s="34">
+      <c r="Q39" s="33">
         <v>7.7999999999999999E-5</v>
       </c>
-      <c r="R39" s="34">
+      <c r="R39" s="33">
         <v>2.9E-5</v>
       </c>
-      <c r="S39" s="35" t="s">
+      <c r="S39" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T39" s="1"/>
@@ -2815,16 +2814,16 @@
       <c r="O40" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P40" s="34">
+      <c r="P40" s="33">
         <v>1.5667800000000001</v>
       </c>
-      <c r="Q40" s="34">
+      <c r="Q40" s="33">
         <v>1.3300000000000001E-4</v>
       </c>
-      <c r="R40" s="34">
+      <c r="R40" s="33">
         <v>-1.11E-4</v>
       </c>
-      <c r="S40" s="35" t="s">
+      <c r="S40" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T40" s="1"/>
@@ -2870,16 +2869,16 @@
       <c r="O41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P41" s="34">
+      <c r="P41" s="33">
         <v>1.580225</v>
       </c>
-      <c r="Q41" s="34">
+      <c r="Q41" s="33">
         <v>1.5999999999999999E-5</v>
       </c>
-      <c r="R41" s="34">
+      <c r="R41" s="33">
         <v>1.56E-4</v>
       </c>
-      <c r="S41" s="35" t="s">
+      <c r="S41" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T41" s="1"/>
@@ -2925,16 +2924,16 @@
       <c r="O42" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P42" s="34">
+      <c r="P42" s="33">
         <v>1.576541</v>
       </c>
-      <c r="Q42" s="34">
+      <c r="Q42" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="R42" s="34">
+      <c r="R42" s="33">
         <v>1.17E-4</v>
       </c>
-      <c r="S42" s="35" t="s">
+      <c r="S42" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T42" s="1"/>
@@ -2980,16 +2979,16 @@
       <c r="O43" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="P43" s="34">
+      <c r="P43" s="33">
         <v>1.5685560000000001</v>
       </c>
-      <c r="Q43" s="34">
+      <c r="Q43" s="33">
         <v>1.83E-4</v>
       </c>
-      <c r="R43" s="34">
+      <c r="R43" s="33">
         <v>1.2999999999999999E-5</v>
       </c>
-      <c r="S43" s="35" t="s">
+      <c r="S43" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T43" s="1"/>
@@ -3035,16 +3034,16 @@
       <c r="O44" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="P44" s="34">
+      <c r="P44" s="33">
         <v>1.568163</v>
       </c>
-      <c r="Q44" s="34">
+      <c r="Q44" s="33">
         <v>-5.1E-5</v>
       </c>
-      <c r="R44" s="34">
+      <c r="R44" s="33">
         <v>-7.1000000000000005E-5</v>
       </c>
-      <c r="S44" s="35" t="s">
+      <c r="S44" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T44" s="1"/>
@@ -3090,16 +3089,16 @@
       <c r="O45" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="P45" s="34">
+      <c r="P45" s="33">
         <v>1.5656429999999999</v>
       </c>
-      <c r="Q45" s="34">
+      <c r="Q45" s="33">
         <v>3.3199999999999999E-4</v>
       </c>
-      <c r="R45" s="34">
+      <c r="R45" s="33">
         <v>1.45E-4</v>
       </c>
-      <c r="S45" s="35" t="s">
+      <c r="S45" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T45" s="1"/>
@@ -3145,16 +3144,16 @@
       <c r="O46" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="P46" s="34">
+      <c r="P46" s="33">
         <v>1.5660339999999999</v>
       </c>
-      <c r="Q46" s="34">
+      <c r="Q46" s="33">
         <v>1.603E-3</v>
       </c>
-      <c r="R46" s="34">
+      <c r="R46" s="33">
         <v>9.1600000000000004E-4</v>
       </c>
-      <c r="S46" s="35" t="s">
+      <c r="S46" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T46" s="1"/>
@@ -3200,16 +3199,16 @@
       <c r="O47" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P47" s="34">
+      <c r="P47" s="33">
         <v>1.5687249999999999</v>
       </c>
-      <c r="Q47" s="34">
+      <c r="Q47" s="33">
         <v>1.8599999999999999E-4</v>
       </c>
-      <c r="R47" s="34">
+      <c r="R47" s="33">
         <v>1.8E-5</v>
       </c>
-      <c r="S47" s="35" t="s">
+      <c r="S47" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T47" s="1"/>
@@ -3255,16 +3254,16 @@
       <c r="O48" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P48" s="34">
+      <c r="P48" s="33">
         <v>1.568155</v>
       </c>
-      <c r="Q48" s="34">
+      <c r="Q48" s="33">
         <v>4.6900000000000002E-4</v>
       </c>
-      <c r="R48" s="34">
+      <c r="R48" s="33">
         <v>2.7700000000000001E-4</v>
       </c>
-      <c r="S48" s="35" t="s">
+      <c r="S48" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T48" s="1"/>
@@ -3310,16 +3309,16 @@
       <c r="O49" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="P49" s="34">
+      <c r="P49" s="33">
         <v>1.57718</v>
       </c>
-      <c r="Q49" s="34">
+      <c r="Q49" s="33">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="R49" s="34">
+      <c r="R49" s="33">
         <v>7.2999999999999999E-5</v>
       </c>
-      <c r="S49" s="35" t="s">
+      <c r="S49" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T49" s="1"/>
@@ -3365,16 +3364,16 @@
       <c r="O50" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P50" s="34">
+      <c r="P50" s="33">
         <v>1.575399</v>
       </c>
-      <c r="Q50" s="34">
+      <c r="Q50" s="33">
         <v>1.15E-4</v>
       </c>
-      <c r="R50" s="34">
+      <c r="R50" s="33">
         <v>5.8E-5</v>
       </c>
-      <c r="S50" s="35" t="s">
+      <c r="S50" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T50" s="1"/>
@@ -3420,16 +3419,16 @@
       <c r="O51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="P51" s="34">
+      <c r="P51" s="33">
         <v>1.566276</v>
       </c>
-      <c r="Q51" s="34">
+      <c r="Q51" s="33">
         <v>5.2999999999999998E-4</v>
       </c>
-      <c r="R51" s="34">
+      <c r="R51" s="33">
         <v>2.2599999999999999E-4</v>
       </c>
-      <c r="S51" s="35" t="s">
+      <c r="S51" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T51" s="1"/>
@@ -3475,16 +3474,16 @@
       <c r="O52" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="P52" s="34">
+      <c r="P52" s="33">
         <v>1.5652330000000001</v>
       </c>
-      <c r="Q52" s="34">
+      <c r="Q52" s="33">
         <v>-7.3999999999999996E-5</v>
       </c>
-      <c r="R52" s="34">
+      <c r="R52" s="33">
         <v>-6.9999999999999994E-5</v>
       </c>
-      <c r="S52" s="35" t="s">
+      <c r="S52" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T52" s="1"/>
@@ -3530,16 +3529,16 @@
       <c r="O53" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="P53" s="34">
+      <c r="P53" s="33">
         <v>1.567515</v>
       </c>
-      <c r="Q53" s="34">
+      <c r="Q53" s="33">
         <v>-7.4999999999999993E-5</v>
       </c>
-      <c r="R53" s="34">
+      <c r="R53" s="33">
         <v>-1.02E-4</v>
       </c>
-      <c r="S53" s="35" t="s">
+      <c r="S53" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T53" s="1"/>
@@ -3585,16 +3584,16 @@
       <c r="O54" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P54" s="34">
+      <c r="P54" s="33">
         <v>1.5672900000000001</v>
       </c>
-      <c r="Q54" s="34">
+      <c r="Q54" s="33">
         <v>2.4399999999999999E-4</v>
       </c>
-      <c r="R54" s="34">
+      <c r="R54" s="33">
         <v>7.8999999999999996E-5</v>
       </c>
-      <c r="S54" s="35" t="s">
+      <c r="S54" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T54" s="1"/>
@@ -3640,16 +3639,16 @@
       <c r="O55" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P55" s="34">
+      <c r="P55" s="33">
         <v>1.568673</v>
       </c>
-      <c r="Q55" s="34">
+      <c r="Q55" s="33">
         <v>-6.9999999999999994E-5</v>
       </c>
-      <c r="R55" s="34">
+      <c r="R55" s="33">
         <v>6.0999999999999999E-5</v>
       </c>
-      <c r="S55" s="35" t="s">
+      <c r="S55" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T55" s="1"/>
@@ -3695,16 +3694,16 @@
       <c r="O56" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P56" s="34">
+      <c r="P56" s="33">
         <v>1.5640069999999999</v>
       </c>
-      <c r="Q56" s="34">
+      <c r="Q56" s="33">
         <v>2.4000000000000001E-5</v>
       </c>
-      <c r="R56" s="34">
+      <c r="R56" s="33">
         <v>-6.3E-5</v>
       </c>
-      <c r="S56" s="35" t="s">
+      <c r="S56" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T56" s="1"/>
@@ -3750,16 +3749,16 @@
       <c r="O57" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="P57" s="34">
+      <c r="P57" s="33">
         <v>1.574308</v>
       </c>
-      <c r="Q57" s="34">
+      <c r="Q57" s="33">
         <v>2.4699999999999999E-4</v>
       </c>
-      <c r="R57" s="34">
+      <c r="R57" s="33">
         <v>-2.6999999999999999E-5</v>
       </c>
-      <c r="S57" s="35" t="s">
+      <c r="S57" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T57" s="1"/>
@@ -3805,16 +3804,16 @@
       <c r="O58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P58" s="34">
+      <c r="P58" s="33">
         <v>1.571477</v>
       </c>
-      <c r="Q58" s="34">
+      <c r="Q58" s="33">
         <v>1.17E-4</v>
       </c>
-      <c r="R58" s="34">
+      <c r="R58" s="33">
         <v>1.5E-5</v>
       </c>
-      <c r="S58" s="35" t="s">
+      <c r="S58" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T58" s="1"/>
@@ -3860,16 +3859,16 @@
       <c r="O59" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="P59" s="34">
+      <c r="P59" s="33">
         <v>1.5659620000000001</v>
       </c>
-      <c r="Q59" s="34">
+      <c r="Q59" s="33">
         <v>1.21E-4</v>
       </c>
-      <c r="R59" s="34">
+      <c r="R59" s="33">
         <v>1.9699999999999999E-4</v>
       </c>
-      <c r="S59" s="35" t="s">
+      <c r="S59" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T59" s="1"/>
@@ -3915,16 +3914,16 @@
       <c r="O60" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P60" s="34">
+      <c r="P60" s="33">
         <v>1.570389</v>
       </c>
-      <c r="Q60" s="34">
+      <c r="Q60" s="33">
         <v>-8.2999999999999998E-5</v>
       </c>
-      <c r="R60" s="34">
+      <c r="R60" s="33">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="S60" s="35" t="s">
+      <c r="S60" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T60" s="1"/>
@@ -3970,16 +3969,16 @@
       <c r="O61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="P61" s="34">
+      <c r="P61" s="33">
         <v>1.581202</v>
       </c>
-      <c r="Q61" s="34">
+      <c r="Q61" s="33">
         <v>1.25E-4</v>
       </c>
-      <c r="R61" s="34">
+      <c r="R61" s="33">
         <v>-9.3999999999999994E-5</v>
       </c>
-      <c r="S61" s="35" t="s">
+      <c r="S61" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T61" s="1"/>
@@ -4025,16 +4024,16 @@
       <c r="O62" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P62" s="34">
+      <c r="P62" s="33">
         <v>1.5869279999999999</v>
       </c>
-      <c r="Q62" s="34">
+      <c r="Q62" s="33">
         <v>1.03E-4</v>
       </c>
-      <c r="R62" s="34">
+      <c r="R62" s="33">
         <v>-1.06E-4</v>
       </c>
-      <c r="S62" s="35" t="s">
+      <c r="S62" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T62" s="1"/>
@@ -4080,16 +4079,16 @@
       <c r="O63" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P63" s="34">
+      <c r="P63" s="33">
         <v>1.563175</v>
       </c>
-      <c r="Q63" s="34">
+      <c r="Q63" s="33">
         <v>1.84E-4</v>
       </c>
-      <c r="R63" s="34">
+      <c r="R63" s="33">
         <v>9.7E-5</v>
       </c>
-      <c r="S63" s="35" t="s">
+      <c r="S63" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T63" s="1"/>
@@ -4135,16 +4134,16 @@
       <c r="O64" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P64" s="34">
+      <c r="P64" s="33">
         <v>1.5716380000000001</v>
       </c>
-      <c r="Q64" s="34">
+      <c r="Q64" s="33">
         <v>6.3599999999999996E-4</v>
       </c>
-      <c r="R64" s="34">
+      <c r="R64" s="33">
         <v>5.7499999999999999E-4</v>
       </c>
-      <c r="S64" s="35" t="s">
+      <c r="S64" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T64" s="1"/>
@@ -4190,16 +4189,16 @@
       <c r="O65" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P65" s="34">
+      <c r="P65" s="33">
         <v>1.5718540000000001</v>
       </c>
-      <c r="Q65" s="34">
+      <c r="Q65" s="33">
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="R65" s="34">
+      <c r="R65" s="33">
         <v>-5.8999999999999998E-5</v>
       </c>
-      <c r="S65" s="35" t="s">
+      <c r="S65" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T65" s="1"/>
@@ -4245,16 +4244,16 @@
       <c r="O66" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="P66" s="34">
+      <c r="P66" s="33">
         <v>1.566087</v>
       </c>
-      <c r="Q66" s="34">
+      <c r="Q66" s="33">
         <v>-6.8999999999999997E-5</v>
       </c>
-      <c r="R66" s="34">
+      <c r="R66" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="S66" s="35" t="s">
+      <c r="S66" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T66" s="1"/>
@@ -4300,16 +4299,16 @@
       <c r="O67" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P67" s="34">
+      <c r="P67" s="33">
         <v>1.5691139999999999</v>
       </c>
-      <c r="Q67" s="34">
+      <c r="Q67" s="33">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="R67" s="34">
+      <c r="R67" s="33">
         <v>4.7600000000000002E-4</v>
       </c>
-      <c r="S67" s="35" t="s">
+      <c r="S67" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T67" s="1"/>
@@ -4355,16 +4354,16 @@
       <c r="O68" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="P68" s="34">
+      <c r="P68" s="33">
         <v>1.5704910000000001</v>
       </c>
-      <c r="Q68" s="34">
+      <c r="Q68" s="33">
         <v>-5.7000000000000003E-5</v>
       </c>
-      <c r="R68" s="34">
+      <c r="R68" s="33">
         <v>-3.9999999999999998E-6</v>
       </c>
-      <c r="S68" s="35" t="s">
+      <c r="S68" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T68" s="1"/>
@@ -4410,16 +4409,16 @@
       <c r="O69" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="P69" s="34">
+      <c r="P69" s="33">
         <v>1.567483</v>
       </c>
-      <c r="Q69" s="34">
+      <c r="Q69" s="33">
         <v>1.1400000000000001E-4</v>
       </c>
-      <c r="R69" s="34">
+      <c r="R69" s="33">
         <v>2.24E-4</v>
       </c>
-      <c r="S69" s="35" t="s">
+      <c r="S69" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T69" s="1"/>
@@ -4465,16 +4464,16 @@
       <c r="O70" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="P70" s="34">
+      <c r="P70" s="33">
         <v>1.5686070000000001</v>
       </c>
-      <c r="Q70" s="34">
+      <c r="Q70" s="33">
         <v>3.6600000000000001E-4</v>
       </c>
-      <c r="R70" s="34">
+      <c r="R70" s="33">
         <v>2.8899999999999998E-4</v>
       </c>
-      <c r="S70" s="35" t="s">
+      <c r="S70" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T70" s="1"/>
@@ -4520,16 +4519,16 @@
       <c r="O71" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P71" s="34">
+      <c r="P71" s="33">
         <v>1.5712919999999999</v>
       </c>
-      <c r="Q71" s="34">
+      <c r="Q71" s="33">
         <v>8.7999999999999998E-5</v>
       </c>
-      <c r="R71" s="34">
+      <c r="R71" s="33">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="S71" s="35" t="s">
+      <c r="S71" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T71" s="1"/>
@@ -4575,16 +4574,16 @@
       <c r="O72" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="P72" s="34">
+      <c r="P72" s="33">
         <v>1.569256</v>
       </c>
-      <c r="Q72" s="34">
+      <c r="Q72" s="33">
         <v>1.02E-4</v>
       </c>
-      <c r="R72" s="34">
+      <c r="R72" s="33">
         <v>-2.4000000000000001E-5</v>
       </c>
-      <c r="S72" s="35" t="s">
+      <c r="S72" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T72" s="1"/>
@@ -4630,16 +4629,16 @@
       <c r="O73" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P73" s="34">
+      <c r="P73" s="33">
         <v>1.582989</v>
       </c>
-      <c r="Q73" s="34">
+      <c r="Q73" s="33">
         <v>-2.0999999999999999E-5</v>
       </c>
-      <c r="R73" s="34">
+      <c r="R73" s="33">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="S73" s="35" t="s">
+      <c r="S73" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T73" s="1"/>
@@ -4685,16 +4684,16 @@
       <c r="O74" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="P74" s="34">
+      <c r="P74" s="33">
         <v>1.5741799999999999</v>
       </c>
-      <c r="Q74" s="34">
+      <c r="Q74" s="33">
         <v>-6.0000000000000002E-6</v>
       </c>
-      <c r="R74" s="34">
+      <c r="R74" s="33">
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="S74" s="35" t="s">
+      <c r="S74" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T74" s="1"/>
@@ -4740,16 +4739,16 @@
       <c r="O75" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="P75" s="34">
+      <c r="P75" s="33">
         <v>1.5728519999999999</v>
       </c>
-      <c r="Q75" s="34">
+      <c r="Q75" s="33">
         <v>-7.3999999999999996E-5</v>
       </c>
-      <c r="R75" s="34">
+      <c r="R75" s="33">
         <v>8.3999999999999995E-5</v>
       </c>
-      <c r="S75" s="35" t="s">
+      <c r="S75" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T75" s="1"/>
@@ -4795,16 +4794,16 @@
       <c r="O76" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="P76" s="34">
+      <c r="P76" s="33">
         <v>1.5762640000000001</v>
       </c>
-      <c r="Q76" s="34">
+      <c r="Q76" s="33">
         <v>-6.8999999999999997E-5</v>
       </c>
-      <c r="R76" s="34">
+      <c r="R76" s="33">
         <v>5.3999999999999998E-5</v>
       </c>
-      <c r="S76" s="35" t="s">
+      <c r="S76" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T76" s="1"/>
@@ -4850,16 +4849,16 @@
       <c r="O77" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="P77" s="34">
+      <c r="P77" s="33">
         <v>1.5869960000000001</v>
       </c>
-      <c r="Q77" s="34">
+      <c r="Q77" s="33">
         <v>5.5999999999999999E-5</v>
       </c>
-      <c r="R77" s="34">
+      <c r="R77" s="33">
         <v>1.4300000000000001E-4</v>
       </c>
-      <c r="S77" s="35" t="s">
+      <c r="S77" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T77" s="1"/>
@@ -4905,16 +4904,16 @@
       <c r="O78" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="P78" s="34">
+      <c r="P78" s="33">
         <v>1.5863309999999999</v>
       </c>
-      <c r="Q78" s="34">
+      <c r="Q78" s="33">
         <v>1.227E-3</v>
       </c>
-      <c r="R78" s="34">
+      <c r="R78" s="33">
         <v>1.0870000000000001E-3</v>
       </c>
-      <c r="S78" s="35" t="s">
+      <c r="S78" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T78" s="1"/>
@@ -4960,16 +4959,16 @@
       <c r="O79" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P79" s="34">
+      <c r="P79" s="33">
         <v>1.5712619999999999</v>
       </c>
-      <c r="Q79" s="34">
+      <c r="Q79" s="33">
         <v>4.8999999999999998E-5</v>
       </c>
-      <c r="R79" s="34">
+      <c r="R79" s="33">
         <v>-1.06E-4</v>
       </c>
-      <c r="S79" s="35" t="s">
+      <c r="S79" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T79" s="1"/>
@@ -5015,16 +5014,16 @@
       <c r="O80" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="P80" s="34">
+      <c r="P80" s="33">
         <v>1.5712619999999999</v>
       </c>
-      <c r="Q80" s="34">
+      <c r="Q80" s="33">
         <v>2.6280000000000001E-3</v>
       </c>
-      <c r="R80" s="34">
+      <c r="R80" s="33">
         <v>1.1299999999999999E-3</v>
       </c>
-      <c r="S80" s="35" t="s">
+      <c r="S80" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T80" s="1"/>
@@ -5070,16 +5069,16 @@
       <c r="O81" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="P81" s="34">
+      <c r="P81" s="33">
         <v>1.575108</v>
       </c>
-      <c r="Q81" s="34">
+      <c r="Q81" s="33">
         <v>-3.8999999999999999E-5</v>
       </c>
-      <c r="R81" s="34">
+      <c r="R81" s="33">
         <v>1.0900000000000001E-4</v>
       </c>
-      <c r="S81" s="35" t="s">
+      <c r="S81" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T81" s="1"/>
@@ -5125,16 +5124,16 @@
       <c r="O82" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="P82" s="34">
+      <c r="P82" s="33">
         <v>1.574133</v>
       </c>
-      <c r="Q82" s="34">
+      <c r="Q82" s="33">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="R82" s="34">
+      <c r="R82" s="33">
         <v>1.07E-4</v>
       </c>
-      <c r="S82" s="35" t="s">
+      <c r="S82" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T82" s="1"/>
@@ -5180,16 +5179,16 @@
       <c r="O83" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P83" s="34">
+      <c r="P83" s="33">
         <v>1.575682</v>
       </c>
-      <c r="Q83" s="34">
+      <c r="Q83" s="33">
         <v>7.2599999999999997E-4</v>
       </c>
-      <c r="R83" s="34">
+      <c r="R83" s="33">
         <v>3.0200000000000002E-4</v>
       </c>
-      <c r="S83" s="35" t="s">
+      <c r="S83" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T83" s="1"/>
@@ -5235,16 +5234,16 @@
       <c r="O84" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="P84" s="34">
+      <c r="P84" s="33">
         <v>1.5699350000000001</v>
       </c>
-      <c r="Q84" s="34">
+      <c r="Q84" s="33">
         <v>8.5000000000000006E-5</v>
       </c>
-      <c r="R84" s="34">
+      <c r="R84" s="33">
         <v>-1.2999999999999999E-5</v>
       </c>
-      <c r="S84" s="35" t="s">
+      <c r="S84" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T84" s="1"/>
@@ -5290,16 +5289,16 @@
       <c r="O85" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="P85" s="34">
+      <c r="P85" s="33">
         <v>1.5697540000000001</v>
       </c>
-      <c r="Q85" s="34">
+      <c r="Q85" s="33">
         <v>-3.0000000000000001E-5</v>
       </c>
-      <c r="R85" s="34">
+      <c r="R85" s="33">
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="S85" s="35" t="s">
+      <c r="S85" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T85" s="1"/>
@@ -5345,16 +5344,16 @@
       <c r="O86" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P86" s="34">
+      <c r="P86" s="33">
         <v>1.5617799999999999</v>
       </c>
-      <c r="Q86" s="34">
+      <c r="Q86" s="33">
         <v>-8.7000000000000001E-5</v>
       </c>
-      <c r="R86" s="34">
+      <c r="R86" s="33">
         <v>-8.5000000000000006E-5</v>
       </c>
-      <c r="S86" s="35" t="s">
+      <c r="S86" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T86" s="1"/>
@@ -5400,16 +5399,16 @@
       <c r="O87" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P87" s="34">
+      <c r="P87" s="33">
         <v>1.582557</v>
       </c>
-      <c r="Q87" s="34">
+      <c r="Q87" s="33">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="R87" s="34">
+      <c r="R87" s="33">
         <v>1.47E-4</v>
       </c>
-      <c r="S87" s="35" t="s">
+      <c r="S87" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T87" s="1"/>
@@ -5455,16 +5454,16 @@
       <c r="O88" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="P88" s="34">
+      <c r="P88" s="33">
         <v>1.5629850000000001</v>
       </c>
-      <c r="Q88" s="34">
+      <c r="Q88" s="33">
         <v>-7.8999999999999996E-5</v>
       </c>
-      <c r="R88" s="34">
+      <c r="R88" s="33">
         <v>7.7999999999999999E-5</v>
       </c>
-      <c r="S88" s="35" t="s">
+      <c r="S88" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T88" s="1"/>
@@ -5510,16 +5509,16 @@
       <c r="O89" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="P89" s="34">
+      <c r="P89" s="33">
         <v>1.566656</v>
       </c>
-      <c r="Q89" s="34">
+      <c r="Q89" s="33">
         <v>-9.5000000000000005E-5</v>
       </c>
-      <c r="R89" s="34">
+      <c r="R89" s="33">
         <v>9.2E-5</v>
       </c>
-      <c r="S89" s="35" t="s">
+      <c r="S89" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T89" s="1"/>
@@ -5565,16 +5564,16 @@
       <c r="O90" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="P90" s="34">
+      <c r="P90" s="33">
         <v>1.584387</v>
       </c>
-      <c r="Q90" s="34">
+      <c r="Q90" s="33">
         <v>4.8000000000000001E-5</v>
       </c>
-      <c r="R90" s="34">
+      <c r="R90" s="33">
         <v>-6.7999999999999999E-5</v>
       </c>
-      <c r="S90" s="35" t="s">
+      <c r="S90" s="34" t="s">
         <v>40</v>
       </c>
       <c r="T90" s="1"/>
@@ -5594,10 +5593,10 @@
       <c r="L91" s="5"/>
       <c r="M91" s="8"/>
       <c r="O91" s="4"/>
-      <c r="P91" s="34"/>
-      <c r="Q91" s="34"/>
-      <c r="R91" s="34"/>
-      <c r="S91" s="35"/>
+      <c r="P91" s="33"/>
+      <c r="Q91" s="33"/>
+      <c r="R91" s="33"/>
+      <c r="S91" s="34"/>
       <c r="T91" s="1"/>
       <c r="V91" s="3"/>
     </row>
@@ -5640,7 +5639,7 @@
         <v>29.340050000000002</v>
       </c>
       <c r="M92" s="14"/>
-      <c r="N92" s="15"/>
+      <c r="N92" s="35"/>
       <c r="O92" s="10"/>
       <c r="P92" s="13">
         <f>AVERAGE(P10:P91)</f>
@@ -5697,7 +5696,7 @@
         <v>28.315799999999999</v>
       </c>
       <c r="M93" s="14"/>
-      <c r="N93" s="15"/>
+      <c r="N93" s="35"/>
       <c r="O93" s="10"/>
       <c r="P93" s="13">
         <f>MIN(P10:P91)</f>
@@ -5754,7 +5753,7 @@
         <v>29.945799999999998</v>
       </c>
       <c r="M94" s="14"/>
-      <c r="N94" s="15"/>
+      <c r="N94" s="35"/>
       <c r="O94" s="10"/>
       <c r="P94" s="13">
         <f>MAX(P10:P91)</f>
@@ -5786,10 +5785,10 @@
       <c r="L95" s="5"/>
       <c r="M95" s="8"/>
       <c r="O95" s="4"/>
-      <c r="P95" s="34"/>
-      <c r="Q95" s="34"/>
-      <c r="R95" s="34"/>
-      <c r="S95" s="35"/>
+      <c r="P95" s="33"/>
+      <c r="Q95" s="33"/>
+      <c r="R95" s="33"/>
+      <c r="S95" s="34"/>
       <c r="T95" s="1"/>
       <c r="V95" s="3"/>
     </row>
@@ -5807,10 +5806,10 @@
       <c r="L96" s="5"/>
       <c r="M96" s="8"/>
       <c r="O96" s="4"/>
-      <c r="P96" s="34"/>
-      <c r="Q96" s="34"/>
-      <c r="R96" s="34"/>
-      <c r="S96" s="35"/>
+      <c r="P96" s="33"/>
+      <c r="Q96" s="33"/>
+      <c r="R96" s="33"/>
+      <c r="S96" s="34"/>
       <c r="T96" s="1"/>
       <c r="V96" s="3"/>
     </row>
@@ -5828,10 +5827,10 @@
       <c r="L97" s="5"/>
       <c r="M97" s="8"/>
       <c r="O97" s="4"/>
-      <c r="P97" s="34"/>
-      <c r="Q97" s="34"/>
-      <c r="R97" s="34"/>
-      <c r="S97" s="35"/>
+      <c r="P97" s="33"/>
+      <c r="Q97" s="33"/>
+      <c r="R97" s="33"/>
+      <c r="S97" s="34"/>
       <c r="T97" s="1"/>
       <c r="V97" s="3"/>
     </row>
@@ -5849,10 +5848,10 @@
       <c r="L98" s="5"/>
       <c r="M98" s="8"/>
       <c r="O98" s="4"/>
-      <c r="P98" s="34"/>
-      <c r="Q98" s="34"/>
-      <c r="R98" s="34"/>
-      <c r="S98" s="35"/>
+      <c r="P98" s="33"/>
+      <c r="Q98" s="33"/>
+      <c r="R98" s="33"/>
+      <c r="S98" s="34"/>
       <c r="T98" s="1"/>
       <c r="V98" s="3"/>
     </row>
@@ -5870,10 +5869,10 @@
       <c r="L99" s="5"/>
       <c r="M99" s="8"/>
       <c r="O99" s="4"/>
-      <c r="P99" s="34"/>
-      <c r="Q99" s="34"/>
-      <c r="R99" s="34"/>
-      <c r="S99" s="35"/>
+      <c r="P99" s="33"/>
+      <c r="Q99" s="33"/>
+      <c r="R99" s="33"/>
+      <c r="S99" s="34"/>
       <c r="T99" s="1"/>
       <c r="V99" s="3"/>
     </row>
@@ -5891,10 +5890,10 @@
       <c r="L100" s="5"/>
       <c r="M100" s="8"/>
       <c r="O100" s="4"/>
-      <c r="P100" s="34"/>
-      <c r="Q100" s="34"/>
-      <c r="R100" s="34"/>
-      <c r="S100" s="35"/>
+      <c r="P100" s="33"/>
+      <c r="Q100" s="33"/>
+      <c r="R100" s="33"/>
+      <c r="S100" s="34"/>
       <c r="T100" s="1"/>
       <c r="V100" s="3"/>
     </row>
@@ -5912,10 +5911,10 @@
       <c r="L101" s="5"/>
       <c r="M101" s="8"/>
       <c r="O101" s="4"/>
-      <c r="P101" s="34"/>
-      <c r="Q101" s="34"/>
-      <c r="R101" s="34"/>
-      <c r="S101" s="35"/>
+      <c r="P101" s="33"/>
+      <c r="Q101" s="33"/>
+      <c r="R101" s="33"/>
+      <c r="S101" s="34"/>
       <c r="T101" s="1"/>
       <c r="V101" s="3"/>
     </row>
@@ -5933,10 +5932,10 @@
       <c r="L102" s="5"/>
       <c r="M102" s="8"/>
       <c r="O102" s="4"/>
-      <c r="P102" s="34"/>
-      <c r="Q102" s="34"/>
-      <c r="R102" s="34"/>
-      <c r="S102" s="35"/>
+      <c r="P102" s="33"/>
+      <c r="Q102" s="33"/>
+      <c r="R102" s="33"/>
+      <c r="S102" s="34"/>
       <c r="T102" s="1"/>
       <c r="V102" s="3"/>
     </row>
@@ -5954,10 +5953,10 @@
       <c r="L103" s="5"/>
       <c r="M103" s="8"/>
       <c r="O103" s="4"/>
-      <c r="P103" s="34"/>
-      <c r="Q103" s="34"/>
-      <c r="R103" s="34"/>
-      <c r="S103" s="35"/>
+      <c r="P103" s="33"/>
+      <c r="Q103" s="33"/>
+      <c r="R103" s="33"/>
+      <c r="S103" s="34"/>
       <c r="T103" s="1"/>
       <c r="V103" s="3"/>
     </row>
@@ -5975,10 +5974,10 @@
       <c r="L104" s="5"/>
       <c r="M104" s="8"/>
       <c r="O104" s="4"/>
-      <c r="P104" s="34"/>
-      <c r="Q104" s="34"/>
-      <c r="R104" s="34"/>
-      <c r="S104" s="35"/>
+      <c r="P104" s="33"/>
+      <c r="Q104" s="33"/>
+      <c r="R104" s="33"/>
+      <c r="S104" s="34"/>
       <c r="T104" s="1"/>
       <c r="V104" s="3"/>
     </row>
@@ -5996,10 +5995,10 @@
       <c r="L105" s="5"/>
       <c r="M105" s="8"/>
       <c r="O105" s="4"/>
-      <c r="P105" s="34"/>
-      <c r="Q105" s="34"/>
-      <c r="R105" s="34"/>
-      <c r="S105" s="35"/>
+      <c r="P105" s="33"/>
+      <c r="Q105" s="33"/>
+      <c r="R105" s="33"/>
+      <c r="S105" s="34"/>
       <c r="T105" s="1"/>
       <c r="V105" s="3"/>
     </row>
@@ -6017,10 +6016,10 @@
       <c r="L106" s="5"/>
       <c r="M106" s="8"/>
       <c r="O106" s="4"/>
-      <c r="P106" s="34"/>
-      <c r="Q106" s="34"/>
-      <c r="R106" s="34"/>
-      <c r="S106" s="35"/>
+      <c r="P106" s="33"/>
+      <c r="Q106" s="33"/>
+      <c r="R106" s="33"/>
+      <c r="S106" s="34"/>
       <c r="T106" s="1"/>
       <c r="V106" s="3"/>
     </row>
@@ -6038,10 +6037,10 @@
       <c r="L107" s="5"/>
       <c r="M107" s="8"/>
       <c r="O107" s="4"/>
-      <c r="P107" s="34"/>
-      <c r="Q107" s="34"/>
-      <c r="R107" s="34"/>
-      <c r="S107" s="35"/>
+      <c r="P107" s="33"/>
+      <c r="Q107" s="33"/>
+      <c r="R107" s="33"/>
+      <c r="S107" s="34"/>
       <c r="T107" s="1"/>
       <c r="V107" s="3"/>
     </row>
@@ -6059,10 +6058,10 @@
       <c r="L108" s="5"/>
       <c r="M108" s="8"/>
       <c r="O108" s="4"/>
-      <c r="P108" s="34"/>
-      <c r="Q108" s="34"/>
-      <c r="R108" s="34"/>
-      <c r="S108" s="35"/>
+      <c r="P108" s="33"/>
+      <c r="Q108" s="33"/>
+      <c r="R108" s="33"/>
+      <c r="S108" s="34"/>
       <c r="T108" s="1"/>
       <c r="V108" s="3"/>
     </row>
@@ -6080,10 +6079,10 @@
       <c r="L109" s="5"/>
       <c r="M109" s="8"/>
       <c r="O109" s="4"/>
-      <c r="P109" s="34"/>
-      <c r="Q109" s="34"/>
-      <c r="R109" s="34"/>
-      <c r="S109" s="35"/>
+      <c r="P109" s="33"/>
+      <c r="Q109" s="33"/>
+      <c r="R109" s="33"/>
+      <c r="S109" s="34"/>
       <c r="T109" s="1"/>
       <c r="V109" s="3"/>
     </row>
@@ -6101,10 +6100,10 @@
       <c r="L110" s="5"/>
       <c r="M110" s="8"/>
       <c r="O110" s="4"/>
-      <c r="P110" s="34"/>
-      <c r="Q110" s="34"/>
-      <c r="R110" s="34"/>
-      <c r="S110" s="35"/>
+      <c r="P110" s="33"/>
+      <c r="Q110" s="33"/>
+      <c r="R110" s="33"/>
+      <c r="S110" s="34"/>
       <c r="T110" s="1"/>
       <c r="V110" s="3"/>
     </row>
@@ -6122,10 +6121,10 @@
       <c r="L111" s="5"/>
       <c r="M111" s="8"/>
       <c r="O111" s="4"/>
-      <c r="P111" s="34"/>
-      <c r="Q111" s="34"/>
-      <c r="R111" s="34"/>
-      <c r="S111" s="35"/>
+      <c r="P111" s="33"/>
+      <c r="Q111" s="33"/>
+      <c r="R111" s="33"/>
+      <c r="S111" s="34"/>
       <c r="T111" s="1"/>
       <c r="V111" s="3"/>
     </row>
@@ -6143,10 +6142,10 @@
       <c r="L112" s="5"/>
       <c r="M112" s="8"/>
       <c r="O112" s="4"/>
-      <c r="P112" s="34"/>
-      <c r="Q112" s="34"/>
-      <c r="R112" s="34"/>
-      <c r="S112" s="35"/>
+      <c r="P112" s="33"/>
+      <c r="Q112" s="33"/>
+      <c r="R112" s="33"/>
+      <c r="S112" s="34"/>
       <c r="T112" s="1"/>
       <c r="V112" s="3"/>
     </row>
@@ -6164,10 +6163,10 @@
       <c r="L113" s="5"/>
       <c r="M113" s="8"/>
       <c r="O113" s="4"/>
-      <c r="P113" s="34"/>
-      <c r="Q113" s="34"/>
-      <c r="R113" s="34"/>
-      <c r="S113" s="35"/>
+      <c r="P113" s="33"/>
+      <c r="Q113" s="33"/>
+      <c r="R113" s="33"/>
+      <c r="S113" s="34"/>
       <c r="T113" s="1"/>
       <c r="V113" s="3"/>
     </row>
@@ -6185,10 +6184,10 @@
       <c r="L114" s="5"/>
       <c r="M114" s="8"/>
       <c r="O114" s="4"/>
-      <c r="P114" s="34"/>
-      <c r="Q114" s="34"/>
-      <c r="R114" s="34"/>
-      <c r="S114" s="35"/>
+      <c r="P114" s="33"/>
+      <c r="Q114" s="33"/>
+      <c r="R114" s="33"/>
+      <c r="S114" s="34"/>
       <c r="T114" s="1"/>
       <c r="V114" s="3"/>
     </row>
@@ -6206,10 +6205,10 @@
       <c r="L115" s="5"/>
       <c r="M115" s="8"/>
       <c r="O115" s="4"/>
-      <c r="P115" s="34"/>
-      <c r="Q115" s="34"/>
-      <c r="R115" s="34"/>
-      <c r="S115" s="35"/>
+      <c r="P115" s="33"/>
+      <c r="Q115" s="33"/>
+      <c r="R115" s="33"/>
+      <c r="S115" s="34"/>
       <c r="T115" s="1"/>
       <c r="V115" s="3"/>
     </row>
@@ -6227,10 +6226,10 @@
       <c r="L116" s="5"/>
       <c r="M116" s="8"/>
       <c r="O116" s="4"/>
-      <c r="P116" s="34"/>
-      <c r="Q116" s="34"/>
-      <c r="R116" s="34"/>
-      <c r="S116" s="35"/>
+      <c r="P116" s="33"/>
+      <c r="Q116" s="33"/>
+      <c r="R116" s="33"/>
+      <c r="S116" s="34"/>
       <c r="T116" s="1"/>
       <c r="V116" s="3"/>
     </row>
@@ -6248,10 +6247,10 @@
       <c r="L117" s="5"/>
       <c r="M117" s="8"/>
       <c r="O117" s="4"/>
-      <c r="P117" s="34"/>
-      <c r="Q117" s="34"/>
-      <c r="R117" s="34"/>
-      <c r="S117" s="35"/>
+      <c r="P117" s="33"/>
+      <c r="Q117" s="33"/>
+      <c r="R117" s="33"/>
+      <c r="S117" s="34"/>
       <c r="T117" s="1"/>
       <c r="V117" s="3"/>
     </row>
@@ -6269,10 +6268,10 @@
       <c r="L118" s="5"/>
       <c r="M118" s="8"/>
       <c r="O118" s="4"/>
-      <c r="P118" s="34"/>
-      <c r="Q118" s="34"/>
-      <c r="R118" s="34"/>
-      <c r="S118" s="35"/>
+      <c r="P118" s="33"/>
+      <c r="Q118" s="33"/>
+      <c r="R118" s="33"/>
+      <c r="S118" s="34"/>
       <c r="T118" s="1"/>
       <c r="V118" s="3"/>
     </row>
@@ -6290,10 +6289,10 @@
       <c r="L119" s="5"/>
       <c r="M119" s="8"/>
       <c r="O119" s="4"/>
-      <c r="P119" s="34"/>
-      <c r="Q119" s="34"/>
-      <c r="R119" s="34"/>
-      <c r="S119" s="35"/>
+      <c r="P119" s="33"/>
+      <c r="Q119" s="33"/>
+      <c r="R119" s="33"/>
+      <c r="S119" s="34"/>
       <c r="T119" s="1"/>
       <c r="V119" s="3"/>
     </row>
@@ -6311,10 +6310,10 @@
       <c r="L120" s="5"/>
       <c r="M120" s="8"/>
       <c r="O120" s="4"/>
-      <c r="P120" s="34"/>
-      <c r="Q120" s="34"/>
-      <c r="R120" s="34"/>
-      <c r="S120" s="35"/>
+      <c r="P120" s="33"/>
+      <c r="Q120" s="33"/>
+      <c r="R120" s="33"/>
+      <c r="S120" s="34"/>
       <c r="T120" s="1"/>
       <c r="V120" s="3"/>
     </row>
@@ -6332,10 +6331,10 @@
       <c r="L121" s="5"/>
       <c r="M121" s="8"/>
       <c r="O121" s="4"/>
-      <c r="P121" s="34"/>
-      <c r="Q121" s="34"/>
-      <c r="R121" s="34"/>
-      <c r="S121" s="35"/>
+      <c r="P121" s="33"/>
+      <c r="Q121" s="33"/>
+      <c r="R121" s="33"/>
+      <c r="S121" s="34"/>
       <c r="T121" s="1"/>
       <c r="V121" s="3"/>
     </row>
@@ -6353,10 +6352,10 @@
       <c r="L122" s="5"/>
       <c r="M122" s="8"/>
       <c r="O122" s="4"/>
-      <c r="P122" s="34"/>
-      <c r="Q122" s="34"/>
-      <c r="R122" s="34"/>
-      <c r="S122" s="35"/>
+      <c r="P122" s="33"/>
+      <c r="Q122" s="33"/>
+      <c r="R122" s="33"/>
+      <c r="S122" s="34"/>
       <c r="T122" s="1"/>
       <c r="V122" s="3"/>
     </row>
@@ -6374,10 +6373,10 @@
       <c r="L123" s="5"/>
       <c r="M123" s="8"/>
       <c r="O123" s="4"/>
-      <c r="P123" s="34"/>
-      <c r="Q123" s="34"/>
-      <c r="R123" s="34"/>
-      <c r="S123" s="35"/>
+      <c r="P123" s="33"/>
+      <c r="Q123" s="33"/>
+      <c r="R123" s="33"/>
+      <c r="S123" s="34"/>
       <c r="T123" s="1"/>
       <c r="V123" s="3"/>
     </row>
@@ -6395,10 +6394,10 @@
       <c r="L124" s="5"/>
       <c r="M124" s="8"/>
       <c r="O124" s="4"/>
-      <c r="P124" s="34"/>
-      <c r="Q124" s="34"/>
-      <c r="R124" s="34"/>
-      <c r="S124" s="35"/>
+      <c r="P124" s="33"/>
+      <c r="Q124" s="33"/>
+      <c r="R124" s="33"/>
+      <c r="S124" s="34"/>
       <c r="T124" s="1"/>
       <c r="V124" s="3"/>
     </row>
@@ -6416,10 +6415,10 @@
       <c r="L125" s="5"/>
       <c r="M125" s="8"/>
       <c r="O125" s="4"/>
-      <c r="P125" s="34"/>
-      <c r="Q125" s="34"/>
-      <c r="R125" s="34"/>
-      <c r="S125" s="35"/>
+      <c r="P125" s="33"/>
+      <c r="Q125" s="33"/>
+      <c r="R125" s="33"/>
+      <c r="S125" s="34"/>
       <c r="T125" s="1"/>
       <c r="V125" s="3"/>
     </row>
@@ -6437,10 +6436,10 @@
       <c r="L126" s="5"/>
       <c r="M126" s="8"/>
       <c r="O126" s="4"/>
-      <c r="P126" s="34"/>
-      <c r="Q126" s="34"/>
-      <c r="R126" s="34"/>
-      <c r="S126" s="35"/>
+      <c r="P126" s="33"/>
+      <c r="Q126" s="33"/>
+      <c r="R126" s="33"/>
+      <c r="S126" s="34"/>
       <c r="T126" s="1"/>
       <c r="V126" s="3"/>
     </row>
@@ -6458,10 +6457,10 @@
       <c r="L127" s="5"/>
       <c r="M127" s="8"/>
       <c r="O127" s="4"/>
-      <c r="P127" s="34"/>
-      <c r="Q127" s="34"/>
-      <c r="R127" s="34"/>
-      <c r="S127" s="35"/>
+      <c r="P127" s="33"/>
+      <c r="Q127" s="33"/>
+      <c r="R127" s="33"/>
+      <c r="S127" s="34"/>
       <c r="T127" s="1"/>
       <c r="V127" s="3"/>
     </row>
@@ -6479,10 +6478,10 @@
       <c r="L128" s="5"/>
       <c r="M128" s="8"/>
       <c r="O128" s="4"/>
-      <c r="P128" s="34"/>
-      <c r="Q128" s="34"/>
-      <c r="R128" s="34"/>
-      <c r="S128" s="35"/>
+      <c r="P128" s="33"/>
+      <c r="Q128" s="33"/>
+      <c r="R128" s="33"/>
+      <c r="S128" s="34"/>
       <c r="T128" s="1"/>
       <c r="V128" s="3"/>
     </row>
@@ -6500,10 +6499,10 @@
       <c r="L129" s="5"/>
       <c r="M129" s="8"/>
       <c r="O129" s="4"/>
-      <c r="P129" s="34"/>
-      <c r="Q129" s="34"/>
-      <c r="R129" s="34"/>
-      <c r="S129" s="35"/>
+      <c r="P129" s="33"/>
+      <c r="Q129" s="33"/>
+      <c r="R129" s="33"/>
+      <c r="S129" s="34"/>
       <c r="T129" s="1"/>
       <c r="V129" s="3"/>
     </row>
@@ -6521,10 +6520,10 @@
       <c r="L130" s="5"/>
       <c r="M130" s="8"/>
       <c r="O130" s="4"/>
-      <c r="P130" s="34"/>
-      <c r="Q130" s="34"/>
-      <c r="R130" s="34"/>
-      <c r="S130" s="35"/>
+      <c r="P130" s="33"/>
+      <c r="Q130" s="33"/>
+      <c r="R130" s="33"/>
+      <c r="S130" s="34"/>
       <c r="T130" s="1"/>
       <c r="V130" s="3"/>
     </row>
@@ -6542,10 +6541,10 @@
       <c r="L131" s="5"/>
       <c r="M131" s="8"/>
       <c r="O131" s="4"/>
-      <c r="P131" s="34"/>
-      <c r="Q131" s="34"/>
-      <c r="R131" s="34"/>
-      <c r="S131" s="35"/>
+      <c r="P131" s="33"/>
+      <c r="Q131" s="33"/>
+      <c r="R131" s="33"/>
+      <c r="S131" s="34"/>
       <c r="T131" s="1"/>
       <c r="V131" s="3"/>
     </row>
@@ -6563,10 +6562,10 @@
       <c r="L132" s="5"/>
       <c r="M132" s="8"/>
       <c r="O132" s="4"/>
-      <c r="P132" s="34"/>
-      <c r="Q132" s="34"/>
-      <c r="R132" s="34"/>
-      <c r="S132" s="35"/>
+      <c r="P132" s="33"/>
+      <c r="Q132" s="33"/>
+      <c r="R132" s="33"/>
+      <c r="S132" s="34"/>
       <c r="T132" s="1"/>
       <c r="V132" s="3"/>
     </row>
@@ -6584,10 +6583,10 @@
       <c r="L133" s="5"/>
       <c r="M133" s="8"/>
       <c r="O133" s="4"/>
-      <c r="P133" s="34"/>
-      <c r="Q133" s="34"/>
-      <c r="R133" s="34"/>
-      <c r="S133" s="35"/>
+      <c r="P133" s="33"/>
+      <c r="Q133" s="33"/>
+      <c r="R133" s="33"/>
+      <c r="S133" s="34"/>
       <c r="T133" s="1"/>
       <c r="V133" s="3"/>
     </row>
@@ -6605,10 +6604,10 @@
       <c r="L134" s="5"/>
       <c r="M134" s="8"/>
       <c r="O134" s="4"/>
-      <c r="P134" s="34"/>
-      <c r="Q134" s="34"/>
-      <c r="R134" s="34"/>
-      <c r="S134" s="35"/>
+      <c r="P134" s="33"/>
+      <c r="Q134" s="33"/>
+      <c r="R134" s="33"/>
+      <c r="S134" s="34"/>
       <c r="T134" s="1"/>
       <c r="V134" s="3"/>
     </row>
@@ -6626,10 +6625,10 @@
       <c r="L135" s="5"/>
       <c r="M135" s="8"/>
       <c r="O135" s="4"/>
-      <c r="P135" s="34"/>
-      <c r="Q135" s="34"/>
-      <c r="R135" s="34"/>
-      <c r="S135" s="35"/>
+      <c r="P135" s="33"/>
+      <c r="Q135" s="33"/>
+      <c r="R135" s="33"/>
+      <c r="S135" s="34"/>
       <c r="T135" s="1"/>
       <c r="V135" s="3"/>
     </row>
@@ -6647,10 +6646,10 @@
       <c r="L136" s="5"/>
       <c r="M136" s="8"/>
       <c r="O136" s="4"/>
-      <c r="P136" s="34"/>
-      <c r="Q136" s="34"/>
-      <c r="R136" s="34"/>
-      <c r="S136" s="35"/>
+      <c r="P136" s="33"/>
+      <c r="Q136" s="33"/>
+      <c r="R136" s="33"/>
+      <c r="S136" s="34"/>
       <c r="T136" s="1"/>
       <c r="V136" s="3"/>
     </row>
@@ -6668,10 +6667,10 @@
       <c r="L137" s="5"/>
       <c r="M137" s="8"/>
       <c r="O137" s="4"/>
-      <c r="P137" s="34"/>
-      <c r="Q137" s="34"/>
-      <c r="R137" s="34"/>
-      <c r="S137" s="35"/>
+      <c r="P137" s="33"/>
+      <c r="Q137" s="33"/>
+      <c r="R137" s="33"/>
+      <c r="S137" s="34"/>
       <c r="T137" s="1"/>
       <c r="V137" s="3"/>
     </row>
@@ -6689,10 +6688,10 @@
       <c r="L138" s="5"/>
       <c r="M138" s="8"/>
       <c r="O138" s="4"/>
-      <c r="P138" s="34"/>
-      <c r="Q138" s="34"/>
-      <c r="R138" s="34"/>
-      <c r="S138" s="35"/>
+      <c r="P138" s="33"/>
+      <c r="Q138" s="33"/>
+      <c r="R138" s="33"/>
+      <c r="S138" s="34"/>
       <c r="T138" s="1"/>
       <c r="V138" s="3"/>
     </row>
@@ -6710,10 +6709,10 @@
       <c r="L139" s="5"/>
       <c r="M139" s="8"/>
       <c r="O139" s="4"/>
-      <c r="P139" s="34"/>
-      <c r="Q139" s="34"/>
-      <c r="R139" s="34"/>
-      <c r="S139" s="35"/>
+      <c r="P139" s="33"/>
+      <c r="Q139" s="33"/>
+      <c r="R139" s="33"/>
+      <c r="S139" s="34"/>
       <c r="T139" s="1"/>
       <c r="V139" s="3"/>
     </row>
@@ -6731,10 +6730,10 @@
       <c r="L140" s="5"/>
       <c r="M140" s="8"/>
       <c r="O140" s="4"/>
-      <c r="P140" s="34"/>
-      <c r="Q140" s="34"/>
-      <c r="R140" s="34"/>
-      <c r="S140" s="35"/>
+      <c r="P140" s="33"/>
+      <c r="Q140" s="33"/>
+      <c r="R140" s="33"/>
+      <c r="S140" s="34"/>
       <c r="T140" s="1"/>
       <c r="V140" s="3"/>
     </row>
@@ -6752,10 +6751,10 @@
       <c r="L141" s="5"/>
       <c r="M141" s="8"/>
       <c r="O141" s="4"/>
-      <c r="P141" s="34"/>
-      <c r="Q141" s="34"/>
-      <c r="R141" s="34"/>
-      <c r="S141" s="35"/>
+      <c r="P141" s="33"/>
+      <c r="Q141" s="33"/>
+      <c r="R141" s="33"/>
+      <c r="S141" s="34"/>
       <c r="T141" s="1"/>
       <c r="V141" s="3"/>
     </row>
@@ -6773,10 +6772,10 @@
       <c r="L142" s="5"/>
       <c r="M142" s="8"/>
       <c r="O142" s="4"/>
-      <c r="P142" s="34"/>
-      <c r="Q142" s="34"/>
-      <c r="R142" s="34"/>
-      <c r="S142" s="35"/>
+      <c r="P142" s="33"/>
+      <c r="Q142" s="33"/>
+      <c r="R142" s="33"/>
+      <c r="S142" s="34"/>
       <c r="T142" s="1"/>
       <c r="V142" s="3"/>
     </row>
@@ -6794,10 +6793,10 @@
       <c r="L143" s="5"/>
       <c r="M143" s="8"/>
       <c r="O143" s="4"/>
-      <c r="P143" s="34"/>
-      <c r="Q143" s="34"/>
-      <c r="R143" s="34"/>
-      <c r="S143" s="35"/>
+      <c r="P143" s="33"/>
+      <c r="Q143" s="33"/>
+      <c r="R143" s="33"/>
+      <c r="S143" s="34"/>
       <c r="T143" s="1"/>
       <c r="V143" s="3"/>
     </row>
@@ -6815,10 +6814,10 @@
       <c r="L144" s="5"/>
       <c r="M144" s="8"/>
       <c r="O144" s="4"/>
-      <c r="P144" s="34"/>
-      <c r="Q144" s="34"/>
-      <c r="R144" s="34"/>
-      <c r="S144" s="35"/>
+      <c r="P144" s="33"/>
+      <c r="Q144" s="33"/>
+      <c r="R144" s="33"/>
+      <c r="S144" s="34"/>
       <c r="T144" s="1"/>
       <c r="V144" s="3"/>
     </row>
@@ -6836,10 +6835,10 @@
       <c r="L145" s="5"/>
       <c r="M145" s="8"/>
       <c r="O145" s="4"/>
-      <c r="P145" s="34"/>
-      <c r="Q145" s="34"/>
-      <c r="R145" s="34"/>
-      <c r="S145" s="35"/>
+      <c r="P145" s="33"/>
+      <c r="Q145" s="33"/>
+      <c r="R145" s="33"/>
+      <c r="S145" s="34"/>
       <c r="T145" s="1"/>
       <c r="V145" s="3"/>
     </row>
@@ -6857,10 +6856,10 @@
       <c r="L146" s="5"/>
       <c r="M146" s="8"/>
       <c r="O146" s="4"/>
-      <c r="P146" s="34"/>
-      <c r="Q146" s="34"/>
-      <c r="R146" s="34"/>
-      <c r="S146" s="35"/>
+      <c r="P146" s="33"/>
+      <c r="Q146" s="33"/>
+      <c r="R146" s="33"/>
+      <c r="S146" s="34"/>
       <c r="T146" s="1"/>
       <c r="V146" s="3"/>
     </row>
@@ -6878,10 +6877,10 @@
       <c r="L147" s="5"/>
       <c r="M147" s="8"/>
       <c r="O147" s="4"/>
-      <c r="P147" s="34"/>
-      <c r="Q147" s="34"/>
-      <c r="R147" s="34"/>
-      <c r="S147" s="35"/>
+      <c r="P147" s="33"/>
+      <c r="Q147" s="33"/>
+      <c r="R147" s="33"/>
+      <c r="S147" s="34"/>
       <c r="T147" s="1"/>
       <c r="V147" s="3"/>
     </row>
@@ -6899,10 +6898,10 @@
       <c r="L148" s="5"/>
       <c r="M148" s="8"/>
       <c r="O148" s="4"/>
-      <c r="P148" s="34"/>
-      <c r="Q148" s="34"/>
-      <c r="R148" s="34"/>
-      <c r="S148" s="35"/>
+      <c r="P148" s="33"/>
+      <c r="Q148" s="33"/>
+      <c r="R148" s="33"/>
+      <c r="S148" s="34"/>
       <c r="T148" s="1"/>
       <c r="V148" s="3"/>
     </row>
@@ -6920,10 +6919,10 @@
       <c r="L149" s="5"/>
       <c r="M149" s="8"/>
       <c r="O149" s="4"/>
-      <c r="P149" s="34"/>
-      <c r="Q149" s="34"/>
-      <c r="R149" s="34"/>
-      <c r="S149" s="35"/>
+      <c r="P149" s="33"/>
+      <c r="Q149" s="33"/>
+      <c r="R149" s="33"/>
+      <c r="S149" s="34"/>
       <c r="T149" s="1"/>
       <c r="V149" s="3"/>
     </row>
@@ -6941,10 +6940,10 @@
       <c r="L150" s="5"/>
       <c r="M150" s="8"/>
       <c r="O150" s="4"/>
-      <c r="P150" s="34"/>
-      <c r="Q150" s="34"/>
-      <c r="R150" s="34"/>
-      <c r="S150" s="35"/>
+      <c r="P150" s="33"/>
+      <c r="Q150" s="33"/>
+      <c r="R150" s="33"/>
+      <c r="S150" s="34"/>
       <c r="T150" s="1"/>
       <c r="V150" s="3"/>
     </row>
@@ -6962,10 +6961,10 @@
       <c r="L151" s="5"/>
       <c r="M151" s="8"/>
       <c r="O151" s="4"/>
-      <c r="P151" s="34"/>
-      <c r="Q151" s="34"/>
-      <c r="R151" s="34"/>
-      <c r="S151" s="35"/>
+      <c r="P151" s="33"/>
+      <c r="Q151" s="33"/>
+      <c r="R151" s="33"/>
+      <c r="S151" s="34"/>
       <c r="T151" s="1"/>
       <c r="V151" s="3"/>
     </row>
@@ -6983,10 +6982,10 @@
       <c r="L152" s="5"/>
       <c r="M152" s="8"/>
       <c r="O152" s="4"/>
-      <c r="P152" s="34"/>
-      <c r="Q152" s="34"/>
-      <c r="R152" s="34"/>
-      <c r="S152" s="35"/>
+      <c r="P152" s="33"/>
+      <c r="Q152" s="33"/>
+      <c r="R152" s="33"/>
+      <c r="S152" s="34"/>
       <c r="T152" s="1"/>
       <c r="V152" s="3"/>
     </row>
@@ -7004,10 +7003,10 @@
       <c r="L153" s="5"/>
       <c r="M153" s="8"/>
       <c r="O153" s="4"/>
-      <c r="P153" s="34"/>
-      <c r="Q153" s="34"/>
-      <c r="R153" s="34"/>
-      <c r="S153" s="35"/>
+      <c r="P153" s="33"/>
+      <c r="Q153" s="33"/>
+      <c r="R153" s="33"/>
+      <c r="S153" s="34"/>
       <c r="T153" s="1"/>
       <c r="V153" s="3"/>
     </row>
@@ -7025,10 +7024,10 @@
       <c r="L154" s="5"/>
       <c r="M154" s="8"/>
       <c r="O154" s="4"/>
-      <c r="P154" s="34"/>
-      <c r="Q154" s="34"/>
-      <c r="R154" s="34"/>
-      <c r="S154" s="35"/>
+      <c r="P154" s="33"/>
+      <c r="Q154" s="33"/>
+      <c r="R154" s="33"/>
+      <c r="S154" s="34"/>
       <c r="T154" s="1"/>
       <c r="V154" s="3"/>
     </row>
@@ -7046,10 +7045,10 @@
       <c r="L155" s="5"/>
       <c r="M155" s="8"/>
       <c r="O155" s="4"/>
-      <c r="P155" s="34"/>
-      <c r="Q155" s="34"/>
-      <c r="R155" s="34"/>
-      <c r="S155" s="35"/>
+      <c r="P155" s="33"/>
+      <c r="Q155" s="33"/>
+      <c r="R155" s="33"/>
+      <c r="S155" s="34"/>
       <c r="T155" s="1"/>
       <c r="V155" s="3"/>
     </row>
@@ -7067,10 +7066,10 @@
       <c r="L156" s="5"/>
       <c r="M156" s="8"/>
       <c r="O156" s="4"/>
-      <c r="P156" s="34"/>
-      <c r="Q156" s="34"/>
-      <c r="R156" s="34"/>
-      <c r="S156" s="35"/>
+      <c r="P156" s="33"/>
+      <c r="Q156" s="33"/>
+      <c r="R156" s="33"/>
+      <c r="S156" s="34"/>
       <c r="T156" s="1"/>
       <c r="V156" s="3"/>
     </row>
@@ -7088,10 +7087,10 @@
       <c r="L157" s="5"/>
       <c r="M157" s="8"/>
       <c r="O157" s="4"/>
-      <c r="P157" s="34"/>
-      <c r="Q157" s="34"/>
-      <c r="R157" s="34"/>
-      <c r="S157" s="35"/>
+      <c r="P157" s="33"/>
+      <c r="Q157" s="33"/>
+      <c r="R157" s="33"/>
+      <c r="S157" s="34"/>
       <c r="T157" s="1"/>
       <c r="V157" s="3"/>
     </row>
@@ -7109,10 +7108,10 @@
       <c r="L158" s="5"/>
       <c r="M158" s="8"/>
       <c r="O158" s="4"/>
-      <c r="P158" s="34"/>
-      <c r="Q158" s="34"/>
-      <c r="R158" s="34"/>
-      <c r="S158" s="35"/>
+      <c r="P158" s="33"/>
+      <c r="Q158" s="33"/>
+      <c r="R158" s="33"/>
+      <c r="S158" s="34"/>
       <c r="T158" s="1"/>
       <c r="V158" s="3"/>
     </row>
@@ -7130,10 +7129,10 @@
       <c r="L159" s="5"/>
       <c r="M159" s="8"/>
       <c r="O159" s="4"/>
-      <c r="P159" s="34"/>
-      <c r="Q159" s="34"/>
-      <c r="R159" s="34"/>
-      <c r="S159" s="35"/>
+      <c r="P159" s="33"/>
+      <c r="Q159" s="33"/>
+      <c r="R159" s="33"/>
+      <c r="S159" s="34"/>
       <c r="T159" s="1"/>
       <c r="V159" s="3"/>
     </row>
@@ -7151,10 +7150,10 @@
       <c r="L160" s="5"/>
       <c r="M160" s="8"/>
       <c r="O160" s="4"/>
-      <c r="P160" s="34"/>
-      <c r="Q160" s="34"/>
-      <c r="R160" s="34"/>
-      <c r="S160" s="35"/>
+      <c r="P160" s="33"/>
+      <c r="Q160" s="33"/>
+      <c r="R160" s="33"/>
+      <c r="S160" s="34"/>
       <c r="T160" s="1"/>
       <c r="V160" s="3"/>
     </row>
@@ -7172,10 +7171,10 @@
       <c r="L161" s="5"/>
       <c r="M161" s="8"/>
       <c r="O161" s="4"/>
-      <c r="P161" s="34"/>
-      <c r="Q161" s="34"/>
-      <c r="R161" s="34"/>
-      <c r="S161" s="35"/>
+      <c r="P161" s="33"/>
+      <c r="Q161" s="33"/>
+      <c r="R161" s="33"/>
+      <c r="S161" s="34"/>
       <c r="T161" s="1"/>
       <c r="V161" s="3"/>
     </row>
@@ -7193,10 +7192,10 @@
       <c r="L162" s="5"/>
       <c r="M162" s="8"/>
       <c r="O162" s="4"/>
-      <c r="P162" s="34"/>
-      <c r="Q162" s="34"/>
-      <c r="R162" s="34"/>
-      <c r="S162" s="35"/>
+      <c r="P162" s="33"/>
+      <c r="Q162" s="33"/>
+      <c r="R162" s="33"/>
+      <c r="S162" s="34"/>
       <c r="T162" s="1"/>
       <c r="V162" s="3"/>
     </row>
@@ -7214,10 +7213,10 @@
       <c r="L163" s="5"/>
       <c r="M163" s="8"/>
       <c r="O163" s="4"/>
-      <c r="P163" s="34"/>
-      <c r="Q163" s="34"/>
-      <c r="R163" s="34"/>
-      <c r="S163" s="35"/>
+      <c r="P163" s="33"/>
+      <c r="Q163" s="33"/>
+      <c r="R163" s="33"/>
+      <c r="S163" s="34"/>
       <c r="T163" s="1"/>
       <c r="V163" s="3"/>
     </row>
@@ -7235,10 +7234,10 @@
       <c r="L164" s="5"/>
       <c r="M164" s="8"/>
       <c r="O164" s="4"/>
-      <c r="P164" s="34"/>
-      <c r="Q164" s="34"/>
-      <c r="R164" s="34"/>
-      <c r="S164" s="35"/>
+      <c r="P164" s="33"/>
+      <c r="Q164" s="33"/>
+      <c r="R164" s="33"/>
+      <c r="S164" s="34"/>
       <c r="T164" s="1"/>
       <c r="V164" s="3"/>
     </row>
@@ -7256,10 +7255,10 @@
       <c r="L165" s="5"/>
       <c r="M165" s="8"/>
       <c r="O165" s="4"/>
-      <c r="P165" s="34"/>
-      <c r="Q165" s="34"/>
-      <c r="R165" s="34"/>
-      <c r="S165" s="35"/>
+      <c r="P165" s="33"/>
+      <c r="Q165" s="33"/>
+      <c r="R165" s="33"/>
+      <c r="S165" s="34"/>
       <c r="T165" s="1"/>
       <c r="V165" s="3"/>
     </row>
@@ -7277,10 +7276,10 @@
       <c r="L166" s="5"/>
       <c r="M166" s="8"/>
       <c r="O166" s="4"/>
-      <c r="P166" s="34"/>
-      <c r="Q166" s="34"/>
-      <c r="R166" s="34"/>
-      <c r="S166" s="35"/>
+      <c r="P166" s="33"/>
+      <c r="Q166" s="33"/>
+      <c r="R166" s="33"/>
+      <c r="S166" s="34"/>
       <c r="T166" s="1"/>
       <c r="V166" s="3"/>
     </row>
@@ -7298,10 +7297,10 @@
       <c r="L167" s="5"/>
       <c r="M167" s="8"/>
       <c r="O167" s="4"/>
-      <c r="P167" s="34"/>
-      <c r="Q167" s="34"/>
-      <c r="R167" s="34"/>
-      <c r="S167" s="35"/>
+      <c r="P167" s="33"/>
+      <c r="Q167" s="33"/>
+      <c r="R167" s="33"/>
+      <c r="S167" s="34"/>
       <c r="T167" s="1"/>
       <c r="V167" s="3"/>
     </row>
@@ -7319,10 +7318,10 @@
       <c r="L168" s="5"/>
       <c r="M168" s="8"/>
       <c r="O168" s="4"/>
-      <c r="P168" s="34"/>
-      <c r="Q168" s="34"/>
-      <c r="R168" s="34"/>
-      <c r="S168" s="35"/>
+      <c r="P168" s="33"/>
+      <c r="Q168" s="33"/>
+      <c r="R168" s="33"/>
+      <c r="S168" s="34"/>
       <c r="T168" s="1"/>
       <c r="V168" s="3"/>
     </row>
@@ -7340,10 +7339,10 @@
       <c r="L169" s="5"/>
       <c r="M169" s="8"/>
       <c r="O169" s="4"/>
-      <c r="P169" s="34"/>
-      <c r="Q169" s="34"/>
-      <c r="R169" s="34"/>
-      <c r="S169" s="35"/>
+      <c r="P169" s="33"/>
+      <c r="Q169" s="33"/>
+      <c r="R169" s="33"/>
+      <c r="S169" s="34"/>
       <c r="T169" s="1"/>
       <c r="V169" s="3"/>
     </row>
@@ -7361,10 +7360,10 @@
       <c r="L170" s="5"/>
       <c r="M170" s="8"/>
       <c r="O170" s="4"/>
-      <c r="P170" s="34"/>
-      <c r="Q170" s="34"/>
-      <c r="R170" s="34"/>
-      <c r="S170" s="35"/>
+      <c r="P170" s="33"/>
+      <c r="Q170" s="33"/>
+      <c r="R170" s="33"/>
+      <c r="S170" s="34"/>
       <c r="T170" s="1"/>
       <c r="V170" s="3"/>
     </row>
@@ -7382,10 +7381,10 @@
       <c r="L171" s="5"/>
       <c r="M171" s="8"/>
       <c r="O171" s="4"/>
-      <c r="P171" s="34"/>
-      <c r="Q171" s="34"/>
-      <c r="R171" s="34"/>
-      <c r="S171" s="35"/>
+      <c r="P171" s="33"/>
+      <c r="Q171" s="33"/>
+      <c r="R171" s="33"/>
+      <c r="S171" s="34"/>
       <c r="T171" s="1"/>
       <c r="V171" s="3"/>
     </row>
@@ -7403,10 +7402,10 @@
       <c r="L172" s="5"/>
       <c r="M172" s="8"/>
       <c r="O172" s="4"/>
-      <c r="P172" s="34"/>
-      <c r="Q172" s="34"/>
-      <c r="R172" s="34"/>
-      <c r="S172" s="35"/>
+      <c r="P172" s="33"/>
+      <c r="Q172" s="33"/>
+      <c r="R172" s="33"/>
+      <c r="S172" s="34"/>
       <c r="T172" s="1"/>
       <c r="V172" s="3"/>
     </row>
@@ -7424,10 +7423,10 @@
       <c r="L173" s="5"/>
       <c r="M173" s="8"/>
       <c r="O173" s="4"/>
-      <c r="P173" s="34"/>
-      <c r="Q173" s="34"/>
-      <c r="R173" s="34"/>
-      <c r="S173" s="35"/>
+      <c r="P173" s="33"/>
+      <c r="Q173" s="33"/>
+      <c r="R173" s="33"/>
+      <c r="S173" s="34"/>
       <c r="T173" s="1"/>
       <c r="V173" s="3"/>
     </row>
@@ -7445,10 +7444,10 @@
       <c r="L174" s="5"/>
       <c r="M174" s="8"/>
       <c r="O174" s="4"/>
-      <c r="P174" s="34"/>
-      <c r="Q174" s="34"/>
-      <c r="R174" s="34"/>
-      <c r="S174" s="35"/>
+      <c r="P174" s="33"/>
+      <c r="Q174" s="33"/>
+      <c r="R174" s="33"/>
+      <c r="S174" s="34"/>
       <c r="T174" s="1"/>
       <c r="V174" s="3"/>
     </row>
@@ -7466,10 +7465,10 @@
       <c r="L175" s="5"/>
       <c r="M175" s="8"/>
       <c r="O175" s="4"/>
-      <c r="P175" s="34"/>
-      <c r="Q175" s="34"/>
-      <c r="R175" s="34"/>
-      <c r="S175" s="35"/>
+      <c r="P175" s="33"/>
+      <c r="Q175" s="33"/>
+      <c r="R175" s="33"/>
+      <c r="S175" s="34"/>
       <c r="T175" s="1"/>
       <c r="V175" s="3"/>
     </row>
@@ -7487,10 +7486,10 @@
       <c r="L176" s="5"/>
       <c r="M176" s="8"/>
       <c r="O176" s="4"/>
-      <c r="P176" s="34"/>
-      <c r="Q176" s="34"/>
-      <c r="R176" s="34"/>
-      <c r="S176" s="35"/>
+      <c r="P176" s="33"/>
+      <c r="Q176" s="33"/>
+      <c r="R176" s="33"/>
+      <c r="S176" s="34"/>
       <c r="T176" s="1"/>
       <c r="V176" s="3"/>
     </row>
@@ -7508,10 +7507,10 @@
       <c r="L177" s="5"/>
       <c r="M177" s="8"/>
       <c r="O177" s="4"/>
-      <c r="P177" s="34"/>
-      <c r="Q177" s="34"/>
-      <c r="R177" s="34"/>
-      <c r="S177" s="35"/>
+      <c r="P177" s="33"/>
+      <c r="Q177" s="33"/>
+      <c r="R177" s="33"/>
+      <c r="S177" s="34"/>
       <c r="T177" s="1"/>
       <c r="V177" s="3"/>
     </row>
@@ -7529,10 +7528,10 @@
       <c r="L178" s="5"/>
       <c r="M178" s="8"/>
       <c r="O178" s="4"/>
-      <c r="P178" s="34"/>
-      <c r="Q178" s="34"/>
-      <c r="R178" s="34"/>
-      <c r="S178" s="35"/>
+      <c r="P178" s="33"/>
+      <c r="Q178" s="33"/>
+      <c r="R178" s="33"/>
+      <c r="S178" s="34"/>
       <c r="T178" s="1"/>
       <c r="V178" s="3"/>
     </row>
@@ -7550,10 +7549,10 @@
       <c r="L179" s="5"/>
       <c r="M179" s="8"/>
       <c r="O179" s="4"/>
-      <c r="P179" s="34"/>
-      <c r="Q179" s="34"/>
-      <c r="R179" s="34"/>
-      <c r="S179" s="35"/>
+      <c r="P179" s="33"/>
+      <c r="Q179" s="33"/>
+      <c r="R179" s="33"/>
+      <c r="S179" s="34"/>
       <c r="T179" s="1"/>
       <c r="V179" s="3"/>
     </row>
@@ -7571,10 +7570,10 @@
       <c r="L180" s="5"/>
       <c r="M180" s="8"/>
       <c r="O180" s="4"/>
-      <c r="P180" s="34"/>
-      <c r="Q180" s="34"/>
-      <c r="R180" s="34"/>
-      <c r="S180" s="35"/>
+      <c r="P180" s="33"/>
+      <c r="Q180" s="33"/>
+      <c r="R180" s="33"/>
+      <c r="S180" s="34"/>
       <c r="T180" s="1"/>
       <c r="V180" s="3"/>
     </row>
@@ -7592,10 +7591,10 @@
       <c r="L181" s="5"/>
       <c r="M181" s="8"/>
       <c r="O181" s="4"/>
-      <c r="P181" s="34"/>
-      <c r="Q181" s="34"/>
-      <c r="R181" s="34"/>
-      <c r="S181" s="35"/>
+      <c r="P181" s="33"/>
+      <c r="Q181" s="33"/>
+      <c r="R181" s="33"/>
+      <c r="S181" s="34"/>
       <c r="T181" s="1"/>
       <c r="V181" s="3"/>
     </row>
@@ -7613,10 +7612,10 @@
       <c r="L182" s="5"/>
       <c r="M182" s="8"/>
       <c r="O182" s="4"/>
-      <c r="P182" s="34"/>
-      <c r="Q182" s="34"/>
-      <c r="R182" s="34"/>
-      <c r="S182" s="35"/>
+      <c r="P182" s="33"/>
+      <c r="Q182" s="33"/>
+      <c r="R182" s="33"/>
+      <c r="S182" s="34"/>
       <c r="T182" s="1"/>
       <c r="V182" s="3"/>
     </row>
@@ -7634,10 +7633,10 @@
       <c r="L183" s="5"/>
       <c r="M183" s="8"/>
       <c r="O183" s="4"/>
-      <c r="P183" s="34"/>
-      <c r="Q183" s="34"/>
-      <c r="R183" s="34"/>
-      <c r="S183" s="35"/>
+      <c r="P183" s="33"/>
+      <c r="Q183" s="33"/>
+      <c r="R183" s="33"/>
+      <c r="S183" s="34"/>
       <c r="T183" s="1"/>
       <c r="V183" s="3"/>
     </row>
@@ -7655,10 +7654,10 @@
       <c r="L184" s="5"/>
       <c r="M184" s="8"/>
       <c r="O184" s="4"/>
-      <c r="P184" s="34"/>
-      <c r="Q184" s="34"/>
-      <c r="R184" s="34"/>
-      <c r="S184" s="35"/>
+      <c r="P184" s="33"/>
+      <c r="Q184" s="33"/>
+      <c r="R184" s="33"/>
+      <c r="S184" s="34"/>
       <c r="T184" s="1"/>
       <c r="V184" s="3"/>
     </row>
@@ -7676,10 +7675,10 @@
       <c r="L185" s="5"/>
       <c r="M185" s="8"/>
       <c r="O185" s="4"/>
-      <c r="P185" s="34"/>
-      <c r="Q185" s="34"/>
-      <c r="R185" s="34"/>
-      <c r="S185" s="35"/>
+      <c r="P185" s="33"/>
+      <c r="Q185" s="33"/>
+      <c r="R185" s="33"/>
+      <c r="S185" s="34"/>
       <c r="T185" s="1"/>
       <c r="V185" s="3"/>
     </row>
@@ -7697,10 +7696,10 @@
       <c r="L186" s="5"/>
       <c r="M186" s="8"/>
       <c r="O186" s="4"/>
-      <c r="P186" s="34"/>
-      <c r="Q186" s="34"/>
-      <c r="R186" s="34"/>
-      <c r="S186" s="35"/>
+      <c r="P186" s="33"/>
+      <c r="Q186" s="33"/>
+      <c r="R186" s="33"/>
+      <c r="S186" s="34"/>
       <c r="T186" s="1"/>
       <c r="V186" s="3"/>
     </row>
@@ -7718,10 +7717,10 @@
       <c r="L187" s="5"/>
       <c r="M187" s="8"/>
       <c r="O187" s="4"/>
-      <c r="P187" s="34"/>
-      <c r="Q187" s="34"/>
-      <c r="R187" s="34"/>
-      <c r="S187" s="35"/>
+      <c r="P187" s="33"/>
+      <c r="Q187" s="33"/>
+      <c r="R187" s="33"/>
+      <c r="S187" s="34"/>
       <c r="T187" s="1"/>
       <c r="V187" s="3"/>
     </row>
@@ -7739,10 +7738,10 @@
       <c r="L188" s="5"/>
       <c r="M188" s="8"/>
       <c r="O188" s="4"/>
-      <c r="P188" s="34"/>
-      <c r="Q188" s="34"/>
-      <c r="R188" s="34"/>
-      <c r="S188" s="35"/>
+      <c r="P188" s="33"/>
+      <c r="Q188" s="33"/>
+      <c r="R188" s="33"/>
+      <c r="S188" s="34"/>
       <c r="T188" s="1"/>
       <c r="V188" s="3"/>
     </row>
@@ -7760,10 +7759,10 @@
       <c r="L189" s="5"/>
       <c r="M189" s="8"/>
       <c r="O189" s="4"/>
-      <c r="P189" s="34"/>
-      <c r="Q189" s="34"/>
-      <c r="R189" s="34"/>
-      <c r="S189" s="35"/>
+      <c r="P189" s="33"/>
+      <c r="Q189" s="33"/>
+      <c r="R189" s="33"/>
+      <c r="S189" s="34"/>
       <c r="T189" s="1"/>
       <c r="V189" s="3"/>
     </row>
@@ -7781,10 +7780,10 @@
       <c r="L190" s="5"/>
       <c r="M190" s="8"/>
       <c r="O190" s="4"/>
-      <c r="P190" s="34"/>
-      <c r="Q190" s="34"/>
-      <c r="R190" s="34"/>
-      <c r="S190" s="35"/>
+      <c r="P190" s="33"/>
+      <c r="Q190" s="33"/>
+      <c r="R190" s="33"/>
+      <c r="S190" s="34"/>
       <c r="T190" s="1"/>
       <c r="V190" s="3"/>
     </row>
@@ -7802,10 +7801,10 @@
       <c r="L191" s="5"/>
       <c r="M191" s="8"/>
       <c r="O191" s="4"/>
-      <c r="P191" s="34"/>
-      <c r="Q191" s="34"/>
-      <c r="R191" s="34"/>
-      <c r="S191" s="35"/>
+      <c r="P191" s="33"/>
+      <c r="Q191" s="33"/>
+      <c r="R191" s="33"/>
+      <c r="S191" s="34"/>
       <c r="T191" s="1"/>
       <c r="V191" s="3"/>
     </row>
@@ -7823,10 +7822,10 @@
       <c r="L192" s="5"/>
       <c r="M192" s="8"/>
       <c r="O192" s="4"/>
-      <c r="P192" s="34"/>
-      <c r="Q192" s="34"/>
-      <c r="R192" s="34"/>
-      <c r="S192" s="35"/>
+      <c r="P192" s="33"/>
+      <c r="Q192" s="33"/>
+      <c r="R192" s="33"/>
+      <c r="S192" s="34"/>
       <c r="T192" s="1"/>
       <c r="V192" s="3"/>
     </row>
@@ -7844,10 +7843,10 @@
       <c r="L193" s="5"/>
       <c r="M193" s="8"/>
       <c r="O193" s="4"/>
-      <c r="P193" s="34"/>
-      <c r="Q193" s="34"/>
-      <c r="R193" s="34"/>
-      <c r="S193" s="35"/>
+      <c r="P193" s="33"/>
+      <c r="Q193" s="33"/>
+      <c r="R193" s="33"/>
+      <c r="S193" s="34"/>
       <c r="T193" s="1"/>
       <c r="V193" s="3"/>
     </row>
@@ -7865,10 +7864,10 @@
       <c r="L194" s="5"/>
       <c r="M194" s="8"/>
       <c r="O194" s="4"/>
-      <c r="P194" s="34"/>
-      <c r="Q194" s="34"/>
-      <c r="R194" s="34"/>
-      <c r="S194" s="35"/>
+      <c r="P194" s="33"/>
+      <c r="Q194" s="33"/>
+      <c r="R194" s="33"/>
+      <c r="S194" s="34"/>
       <c r="T194" s="1"/>
       <c r="V194" s="3"/>
     </row>
@@ -7886,10 +7885,10 @@
       <c r="L195" s="5"/>
       <c r="M195" s="8"/>
       <c r="O195" s="4"/>
-      <c r="P195" s="34"/>
-      <c r="Q195" s="34"/>
-      <c r="R195" s="34"/>
-      <c r="S195" s="35"/>
+      <c r="P195" s="33"/>
+      <c r="Q195" s="33"/>
+      <c r="R195" s="33"/>
+      <c r="S195" s="34"/>
       <c r="T195" s="1"/>
       <c r="V195" s="3"/>
     </row>
@@ -7907,10 +7906,10 @@
       <c r="L196" s="5"/>
       <c r="M196" s="8"/>
       <c r="O196" s="4"/>
-      <c r="P196" s="34"/>
-      <c r="Q196" s="34"/>
-      <c r="R196" s="34"/>
-      <c r="S196" s="35"/>
+      <c r="P196" s="33"/>
+      <c r="Q196" s="33"/>
+      <c r="R196" s="33"/>
+      <c r="S196" s="34"/>
       <c r="T196" s="1"/>
       <c r="V196" s="3"/>
     </row>
@@ -7928,10 +7927,10 @@
       <c r="L197" s="5"/>
       <c r="M197" s="8"/>
       <c r="O197" s="4"/>
-      <c r="P197" s="34"/>
-      <c r="Q197" s="34"/>
-      <c r="R197" s="34"/>
-      <c r="S197" s="35"/>
+      <c r="P197" s="33"/>
+      <c r="Q197" s="33"/>
+      <c r="R197" s="33"/>
+      <c r="S197" s="34"/>
       <c r="T197" s="1"/>
       <c r="V197" s="3"/>
     </row>
@@ -7949,10 +7948,10 @@
       <c r="L198" s="5"/>
       <c r="M198" s="8"/>
       <c r="O198" s="4"/>
-      <c r="P198" s="34"/>
-      <c r="Q198" s="34"/>
-      <c r="R198" s="34"/>
-      <c r="S198" s="35"/>
+      <c r="P198" s="33"/>
+      <c r="Q198" s="33"/>
+      <c r="R198" s="33"/>
+      <c r="S198" s="34"/>
       <c r="T198" s="1"/>
       <c r="V198" s="3"/>
     </row>
@@ -7970,10 +7969,10 @@
       <c r="L199" s="5"/>
       <c r="M199" s="8"/>
       <c r="O199" s="4"/>
-      <c r="P199" s="34"/>
-      <c r="Q199" s="34"/>
-      <c r="R199" s="34"/>
-      <c r="S199" s="35"/>
+      <c r="P199" s="33"/>
+      <c r="Q199" s="33"/>
+      <c r="R199" s="33"/>
+      <c r="S199" s="34"/>
       <c r="T199" s="1"/>
       <c r="V199" s="3"/>
     </row>
@@ -7991,10 +7990,10 @@
       <c r="L200" s="5"/>
       <c r="M200" s="8"/>
       <c r="O200" s="4"/>
-      <c r="P200" s="34"/>
-      <c r="Q200" s="34"/>
-      <c r="R200" s="34"/>
-      <c r="S200" s="35"/>
+      <c r="P200" s="33"/>
+      <c r="Q200" s="33"/>
+      <c r="R200" s="33"/>
+      <c r="S200" s="34"/>
       <c r="T200" s="1"/>
       <c r="V200" s="3"/>
     </row>
@@ -8012,10 +8011,10 @@
       <c r="L201" s="5"/>
       <c r="M201" s="8"/>
       <c r="O201" s="4"/>
-      <c r="P201" s="34"/>
-      <c r="Q201" s="34"/>
-      <c r="R201" s="34"/>
-      <c r="S201" s="35"/>
+      <c r="P201" s="33"/>
+      <c r="Q201" s="33"/>
+      <c r="R201" s="33"/>
+      <c r="S201" s="34"/>
       <c r="T201" s="1"/>
       <c r="V201" s="3"/>
     </row>
@@ -8033,10 +8032,10 @@
       <c r="L202" s="5"/>
       <c r="M202" s="8"/>
       <c r="O202" s="4"/>
-      <c r="P202" s="34"/>
-      <c r="Q202" s="34"/>
-      <c r="R202" s="34"/>
-      <c r="S202" s="35"/>
+      <c r="P202" s="33"/>
+      <c r="Q202" s="33"/>
+      <c r="R202" s="33"/>
+      <c r="S202" s="34"/>
       <c r="T202" s="1"/>
       <c r="V202" s="3"/>
     </row>
@@ -8054,10 +8053,10 @@
       <c r="L203" s="5"/>
       <c r="M203" s="8"/>
       <c r="O203" s="4"/>
-      <c r="P203" s="34"/>
-      <c r="Q203" s="34"/>
-      <c r="R203" s="34"/>
-      <c r="S203" s="35"/>
+      <c r="P203" s="33"/>
+      <c r="Q203" s="33"/>
+      <c r="R203" s="33"/>
+      <c r="S203" s="34"/>
       <c r="T203" s="1"/>
       <c r="V203" s="3"/>
     </row>
@@ -8075,10 +8074,10 @@
       <c r="L204" s="5"/>
       <c r="M204" s="8"/>
       <c r="O204" s="4"/>
-      <c r="P204" s="34"/>
-      <c r="Q204" s="34"/>
-      <c r="R204" s="34"/>
-      <c r="S204" s="35"/>
+      <c r="P204" s="33"/>
+      <c r="Q204" s="33"/>
+      <c r="R204" s="33"/>
+      <c r="S204" s="34"/>
       <c r="T204" s="1"/>
       <c r="V204" s="3"/>
     </row>
@@ -8096,10 +8095,10 @@
       <c r="L205" s="5"/>
       <c r="M205" s="8"/>
       <c r="O205" s="4"/>
-      <c r="P205" s="34"/>
-      <c r="Q205" s="34"/>
-      <c r="R205" s="34"/>
-      <c r="S205" s="35"/>
+      <c r="P205" s="33"/>
+      <c r="Q205" s="33"/>
+      <c r="R205" s="33"/>
+      <c r="S205" s="34"/>
       <c r="T205" s="1"/>
       <c r="V205" s="3"/>
     </row>
@@ -8117,10 +8116,10 @@
       <c r="L206" s="5"/>
       <c r="M206" s="8"/>
       <c r="O206" s="4"/>
-      <c r="P206" s="34"/>
-      <c r="Q206" s="34"/>
-      <c r="R206" s="34"/>
-      <c r="S206" s="35"/>
+      <c r="P206" s="33"/>
+      <c r="Q206" s="33"/>
+      <c r="R206" s="33"/>
+      <c r="S206" s="34"/>
       <c r="T206" s="1"/>
       <c r="V206" s="3"/>
     </row>
@@ -8138,10 +8137,10 @@
       <c r="L207" s="5"/>
       <c r="M207" s="8"/>
       <c r="O207" s="4"/>
-      <c r="P207" s="34"/>
-      <c r="Q207" s="34"/>
-      <c r="R207" s="34"/>
-      <c r="S207" s="35"/>
+      <c r="P207" s="33"/>
+      <c r="Q207" s="33"/>
+      <c r="R207" s="33"/>
+      <c r="S207" s="34"/>
       <c r="T207" s="1"/>
       <c r="V207" s="3"/>
     </row>
@@ -8159,10 +8158,10 @@
       <c r="L208" s="5"/>
       <c r="M208" s="8"/>
       <c r="O208" s="4"/>
-      <c r="P208" s="34"/>
-      <c r="Q208" s="34"/>
-      <c r="R208" s="34"/>
-      <c r="S208" s="35"/>
+      <c r="P208" s="33"/>
+      <c r="Q208" s="33"/>
+      <c r="R208" s="33"/>
+      <c r="S208" s="34"/>
       <c r="T208" s="1"/>
       <c r="V208" s="3"/>
     </row>
@@ -8180,10 +8179,10 @@
       <c r="L209" s="5"/>
       <c r="M209" s="8"/>
       <c r="O209" s="4"/>
-      <c r="P209" s="34"/>
-      <c r="Q209" s="34"/>
-      <c r="R209" s="34"/>
-      <c r="S209" s="35"/>
+      <c r="P209" s="33"/>
+      <c r="Q209" s="33"/>
+      <c r="R209" s="33"/>
+      <c r="S209" s="34"/>
       <c r="T209" s="1"/>
       <c r="V209" s="3"/>
     </row>
@@ -8201,10 +8200,10 @@
       <c r="L210" s="5"/>
       <c r="M210" s="8"/>
       <c r="O210" s="4"/>
-      <c r="P210" s="34"/>
-      <c r="Q210" s="34"/>
-      <c r="R210" s="34"/>
-      <c r="S210" s="35"/>
+      <c r="P210" s="33"/>
+      <c r="Q210" s="33"/>
+      <c r="R210" s="33"/>
+      <c r="S210" s="34"/>
       <c r="T210" s="1"/>
       <c r="V210" s="3"/>
     </row>
@@ -8222,10 +8221,10 @@
       <c r="L211" s="5"/>
       <c r="M211" s="8"/>
       <c r="O211" s="4"/>
-      <c r="P211" s="34"/>
-      <c r="Q211" s="34"/>
-      <c r="R211" s="34"/>
-      <c r="S211" s="35"/>
+      <c r="P211" s="33"/>
+      <c r="Q211" s="33"/>
+      <c r="R211" s="33"/>
+      <c r="S211" s="34"/>
       <c r="T211" s="1"/>
       <c r="V211" s="3"/>
     </row>
@@ -8243,10 +8242,10 @@
       <c r="L212" s="5"/>
       <c r="M212" s="8"/>
       <c r="O212" s="4"/>
-      <c r="P212" s="34"/>
-      <c r="Q212" s="34"/>
-      <c r="R212" s="34"/>
-      <c r="S212" s="35"/>
+      <c r="P212" s="33"/>
+      <c r="Q212" s="33"/>
+      <c r="R212" s="33"/>
+      <c r="S212" s="34"/>
       <c r="T212" s="1"/>
       <c r="V212" s="3"/>
     </row>
@@ -8264,10 +8263,10 @@
       <c r="L213" s="5"/>
       <c r="M213" s="8"/>
       <c r="O213" s="4"/>
-      <c r="P213" s="34"/>
-      <c r="Q213" s="34"/>
-      <c r="R213" s="34"/>
-      <c r="S213" s="35"/>
+      <c r="P213" s="33"/>
+      <c r="Q213" s="33"/>
+      <c r="R213" s="33"/>
+      <c r="S213" s="34"/>
       <c r="T213" s="1"/>
       <c r="V213" s="3"/>
     </row>
@@ -8285,10 +8284,10 @@
       <c r="L214" s="5"/>
       <c r="M214" s="8"/>
       <c r="O214" s="4"/>
-      <c r="P214" s="34"/>
-      <c r="Q214" s="34"/>
-      <c r="R214" s="34"/>
-      <c r="S214" s="35"/>
+      <c r="P214" s="33"/>
+      <c r="Q214" s="33"/>
+      <c r="R214" s="33"/>
+      <c r="S214" s="34"/>
       <c r="T214" s="1"/>
       <c r="V214" s="3"/>
     </row>
@@ -8306,10 +8305,10 @@
       <c r="L215" s="5"/>
       <c r="M215" s="8"/>
       <c r="O215" s="4"/>
-      <c r="P215" s="34"/>
-      <c r="Q215" s="34"/>
-      <c r="R215" s="34"/>
-      <c r="S215" s="35"/>
+      <c r="P215" s="33"/>
+      <c r="Q215" s="33"/>
+      <c r="R215" s="33"/>
+      <c r="S215" s="34"/>
       <c r="T215" s="1"/>
       <c r="V215" s="3"/>
     </row>
@@ -8327,10 +8326,10 @@
       <c r="L216" s="5"/>
       <c r="M216" s="8"/>
       <c r="O216" s="4"/>
-      <c r="P216" s="34"/>
-      <c r="Q216" s="34"/>
-      <c r="R216" s="34"/>
-      <c r="S216" s="35"/>
+      <c r="P216" s="33"/>
+      <c r="Q216" s="33"/>
+      <c r="R216" s="33"/>
+      <c r="S216" s="34"/>
       <c r="T216" s="1"/>
       <c r="V216" s="3"/>
     </row>
@@ -8348,10 +8347,10 @@
       <c r="L217" s="5"/>
       <c r="M217" s="8"/>
       <c r="O217" s="4"/>
-      <c r="P217" s="34"/>
-      <c r="Q217" s="34"/>
-      <c r="R217" s="34"/>
-      <c r="S217" s="35"/>
+      <c r="P217" s="33"/>
+      <c r="Q217" s="33"/>
+      <c r="R217" s="33"/>
+      <c r="S217" s="34"/>
       <c r="T217" s="1"/>
       <c r="V217" s="3"/>
     </row>
@@ -8369,10 +8368,10 @@
       <c r="L218" s="5"/>
       <c r="M218" s="8"/>
       <c r="O218" s="4"/>
-      <c r="P218" s="34"/>
-      <c r="Q218" s="34"/>
-      <c r="R218" s="34"/>
-      <c r="S218" s="35"/>
+      <c r="P218" s="33"/>
+      <c r="Q218" s="33"/>
+      <c r="R218" s="33"/>
+      <c r="S218" s="34"/>
       <c r="T218" s="1"/>
       <c r="V218" s="3"/>
     </row>
@@ -8390,10 +8389,10 @@
       <c r="L219" s="5"/>
       <c r="M219" s="8"/>
       <c r="O219" s="4"/>
-      <c r="P219" s="34"/>
-      <c r="Q219" s="34"/>
-      <c r="R219" s="34"/>
-      <c r="S219" s="35"/>
+      <c r="P219" s="33"/>
+      <c r="Q219" s="33"/>
+      <c r="R219" s="33"/>
+      <c r="S219" s="34"/>
       <c r="T219" s="1"/>
       <c r="V219" s="3"/>
     </row>
@@ -8411,10 +8410,10 @@
       <c r="L220" s="5"/>
       <c r="M220" s="8"/>
       <c r="O220" s="4"/>
-      <c r="P220" s="34"/>
-      <c r="Q220" s="34"/>
-      <c r="R220" s="34"/>
-      <c r="S220" s="35"/>
+      <c r="P220" s="33"/>
+      <c r="Q220" s="33"/>
+      <c r="R220" s="33"/>
+      <c r="S220" s="34"/>
       <c r="T220" s="1"/>
       <c r="V220" s="3"/>
     </row>
@@ -8432,10 +8431,10 @@
       <c r="L221" s="5"/>
       <c r="M221" s="8"/>
       <c r="O221" s="4"/>
-      <c r="P221" s="34"/>
-      <c r="Q221" s="34"/>
-      <c r="R221" s="34"/>
-      <c r="S221" s="35"/>
+      <c r="P221" s="33"/>
+      <c r="Q221" s="33"/>
+      <c r="R221" s="33"/>
+      <c r="S221" s="34"/>
       <c r="T221" s="1"/>
       <c r="V221" s="3"/>
     </row>
@@ -8453,10 +8452,10 @@
       <c r="L222" s="5"/>
       <c r="M222" s="8"/>
       <c r="O222" s="4"/>
-      <c r="P222" s="34"/>
-      <c r="Q222" s="34"/>
-      <c r="R222" s="34"/>
-      <c r="S222" s="35"/>
+      <c r="P222" s="33"/>
+      <c r="Q222" s="33"/>
+      <c r="R222" s="33"/>
+      <c r="S222" s="34"/>
       <c r="T222" s="1"/>
       <c r="V222" s="3"/>
     </row>
@@ -8474,10 +8473,10 @@
       <c r="L223" s="5"/>
       <c r="M223" s="8"/>
       <c r="O223" s="4"/>
-      <c r="P223" s="34"/>
-      <c r="Q223" s="34"/>
-      <c r="R223" s="34"/>
-      <c r="S223" s="35"/>
+      <c r="P223" s="33"/>
+      <c r="Q223" s="33"/>
+      <c r="R223" s="33"/>
+      <c r="S223" s="34"/>
       <c r="T223" s="1"/>
       <c r="V223" s="3"/>
     </row>
@@ -8495,10 +8494,10 @@
       <c r="L224" s="5"/>
       <c r="M224" s="8"/>
       <c r="O224" s="4"/>
-      <c r="P224" s="34"/>
-      <c r="Q224" s="34"/>
-      <c r="R224" s="34"/>
-      <c r="S224" s="35"/>
+      <c r="P224" s="33"/>
+      <c r="Q224" s="33"/>
+      <c r="R224" s="33"/>
+      <c r="S224" s="34"/>
       <c r="T224" s="1"/>
       <c r="V224" s="3"/>
     </row>
@@ -8516,10 +8515,10 @@
       <c r="L225" s="5"/>
       <c r="M225" s="8"/>
       <c r="O225" s="4"/>
-      <c r="P225" s="34"/>
-      <c r="Q225" s="34"/>
-      <c r="R225" s="34"/>
-      <c r="S225" s="35"/>
+      <c r="P225" s="33"/>
+      <c r="Q225" s="33"/>
+      <c r="R225" s="33"/>
+      <c r="S225" s="34"/>
       <c r="T225" s="1"/>
       <c r="V225" s="3"/>
     </row>
@@ -8537,10 +8536,10 @@
       <c r="L226" s="5"/>
       <c r="M226" s="8"/>
       <c r="O226" s="4"/>
-      <c r="P226" s="34"/>
-      <c r="Q226" s="34"/>
-      <c r="R226" s="34"/>
-      <c r="S226" s="35"/>
+      <c r="P226" s="33"/>
+      <c r="Q226" s="33"/>
+      <c r="R226" s="33"/>
+      <c r="S226" s="34"/>
       <c r="T226" s="1"/>
       <c r="V226" s="3"/>
     </row>
@@ -8558,10 +8557,10 @@
       <c r="L227" s="5"/>
       <c r="M227" s="8"/>
       <c r="O227" s="4"/>
-      <c r="P227" s="34"/>
-      <c r="Q227" s="34"/>
-      <c r="R227" s="34"/>
-      <c r="S227" s="35"/>
+      <c r="P227" s="33"/>
+      <c r="Q227" s="33"/>
+      <c r="R227" s="33"/>
+      <c r="S227" s="34"/>
       <c r="T227" s="1"/>
       <c r="V227" s="3"/>
     </row>
@@ -8579,10 +8578,10 @@
       <c r="L228" s="5"/>
       <c r="M228" s="8"/>
       <c r="O228" s="4"/>
-      <c r="P228" s="34"/>
-      <c r="Q228" s="34"/>
-      <c r="R228" s="34"/>
-      <c r="S228" s="35"/>
+      <c r="P228" s="33"/>
+      <c r="Q228" s="33"/>
+      <c r="R228" s="33"/>
+      <c r="S228" s="34"/>
       <c r="T228" s="1"/>
       <c r="V228" s="3"/>
     </row>
@@ -8600,10 +8599,10 @@
       <c r="L229" s="5"/>
       <c r="M229" s="8"/>
       <c r="O229" s="4"/>
-      <c r="P229" s="34"/>
-      <c r="Q229" s="34"/>
-      <c r="R229" s="34"/>
-      <c r="S229" s="35"/>
+      <c r="P229" s="33"/>
+      <c r="Q229" s="33"/>
+      <c r="R229" s="33"/>
+      <c r="S229" s="34"/>
       <c r="T229" s="1"/>
       <c r="V229" s="3"/>
     </row>
@@ -8621,10 +8620,10 @@
       <c r="L230" s="5"/>
       <c r="M230" s="8"/>
       <c r="O230" s="4"/>
-      <c r="P230" s="34"/>
-      <c r="Q230" s="34"/>
-      <c r="R230" s="34"/>
-      <c r="S230" s="35"/>
+      <c r="P230" s="33"/>
+      <c r="Q230" s="33"/>
+      <c r="R230" s="33"/>
+      <c r="S230" s="34"/>
       <c r="T230" s="1"/>
       <c r="V230" s="3"/>
     </row>
@@ -8642,10 +8641,10 @@
       <c r="L231" s="5"/>
       <c r="M231" s="8"/>
       <c r="O231" s="4"/>
-      <c r="P231" s="34"/>
-      <c r="Q231" s="34"/>
-      <c r="R231" s="34"/>
-      <c r="S231" s="35"/>
+      <c r="P231" s="33"/>
+      <c r="Q231" s="33"/>
+      <c r="R231" s="33"/>
+      <c r="S231" s="34"/>
       <c r="T231" s="1"/>
       <c r="V231" s="3"/>
     </row>
@@ -8663,10 +8662,10 @@
       <c r="L232" s="5"/>
       <c r="M232" s="8"/>
       <c r="O232" s="4"/>
-      <c r="P232" s="34"/>
-      <c r="Q232" s="34"/>
-      <c r="R232" s="34"/>
-      <c r="S232" s="35"/>
+      <c r="P232" s="33"/>
+      <c r="Q232" s="33"/>
+      <c r="R232" s="33"/>
+      <c r="S232" s="34"/>
       <c r="T232" s="1"/>
       <c r="V232" s="3"/>
     </row>
@@ -8684,10 +8683,10 @@
       <c r="L233" s="5"/>
       <c r="M233" s="8"/>
       <c r="O233" s="4"/>
-      <c r="P233" s="34"/>
-      <c r="Q233" s="34"/>
-      <c r="R233" s="34"/>
-      <c r="S233" s="35"/>
+      <c r="P233" s="33"/>
+      <c r="Q233" s="33"/>
+      <c r="R233" s="33"/>
+      <c r="S233" s="34"/>
       <c r="T233" s="1"/>
       <c r="V233" s="3"/>
     </row>
@@ -8705,10 +8704,10 @@
       <c r="L234" s="5"/>
       <c r="M234" s="8"/>
       <c r="O234" s="4"/>
-      <c r="P234" s="34"/>
-      <c r="Q234" s="34"/>
-      <c r="R234" s="34"/>
-      <c r="S234" s="35"/>
+      <c r="P234" s="33"/>
+      <c r="Q234" s="33"/>
+      <c r="R234" s="33"/>
+      <c r="S234" s="34"/>
       <c r="T234" s="1"/>
       <c r="V234" s="3"/>
     </row>
@@ -8726,10 +8725,10 @@
       <c r="L235" s="5"/>
       <c r="M235" s="8"/>
       <c r="O235" s="4"/>
-      <c r="P235" s="34"/>
-      <c r="Q235" s="34"/>
-      <c r="R235" s="34"/>
-      <c r="S235" s="35"/>
+      <c r="P235" s="33"/>
+      <c r="Q235" s="33"/>
+      <c r="R235" s="33"/>
+      <c r="S235" s="34"/>
       <c r="T235" s="1"/>
       <c r="V235" s="3"/>
     </row>
@@ -8747,10 +8746,10 @@
       <c r="L236" s="5"/>
       <c r="M236" s="8"/>
       <c r="O236" s="4"/>
-      <c r="P236" s="34"/>
-      <c r="Q236" s="34"/>
-      <c r="R236" s="34"/>
-      <c r="S236" s="35"/>
+      <c r="P236" s="33"/>
+      <c r="Q236" s="33"/>
+      <c r="R236" s="33"/>
+      <c r="S236" s="34"/>
       <c r="T236" s="1"/>
       <c r="V236" s="3"/>
     </row>
@@ -8768,10 +8767,10 @@
       <c r="L237" s="5"/>
       <c r="M237" s="8"/>
       <c r="O237" s="4"/>
-      <c r="P237" s="34"/>
-      <c r="Q237" s="34"/>
-      <c r="R237" s="34"/>
-      <c r="S237" s="35"/>
+      <c r="P237" s="33"/>
+      <c r="Q237" s="33"/>
+      <c r="R237" s="33"/>
+      <c r="S237" s="34"/>
       <c r="T237" s="1"/>
       <c r="V237" s="3"/>
     </row>
@@ -8789,10 +8788,10 @@
       <c r="L238" s="5"/>
       <c r="M238" s="8"/>
       <c r="O238" s="4"/>
-      <c r="P238" s="34"/>
-      <c r="Q238" s="34"/>
-      <c r="R238" s="34"/>
-      <c r="S238" s="35"/>
+      <c r="P238" s="33"/>
+      <c r="Q238" s="33"/>
+      <c r="R238" s="33"/>
+      <c r="S238" s="34"/>
       <c r="T238" s="1"/>
       <c r="V238" s="3"/>
     </row>
@@ -8810,10 +8809,10 @@
       <c r="L239" s="5"/>
       <c r="M239" s="8"/>
       <c r="O239" s="4"/>
-      <c r="P239" s="34"/>
-      <c r="Q239" s="34"/>
-      <c r="R239" s="34"/>
-      <c r="S239" s="35"/>
+      <c r="P239" s="33"/>
+      <c r="Q239" s="33"/>
+      <c r="R239" s="33"/>
+      <c r="S239" s="34"/>
       <c r="T239" s="1"/>
       <c r="V239" s="3"/>
     </row>
@@ -8831,10 +8830,10 @@
       <c r="L240" s="5"/>
       <c r="M240" s="8"/>
       <c r="O240" s="4"/>
-      <c r="P240" s="34"/>
-      <c r="Q240" s="34"/>
-      <c r="R240" s="34"/>
-      <c r="S240" s="35"/>
+      <c r="P240" s="33"/>
+      <c r="Q240" s="33"/>
+      <c r="R240" s="33"/>
+      <c r="S240" s="34"/>
       <c r="T240" s="1"/>
       <c r="V240" s="3"/>
     </row>
@@ -8852,10 +8851,10 @@
       <c r="L241" s="5"/>
       <c r="M241" s="8"/>
       <c r="O241" s="4"/>
-      <c r="P241" s="34"/>
-      <c r="Q241" s="34"/>
-      <c r="R241" s="34"/>
-      <c r="S241" s="35"/>
+      <c r="P241" s="33"/>
+      <c r="Q241" s="33"/>
+      <c r="R241" s="33"/>
+      <c r="S241" s="34"/>
       <c r="T241" s="1"/>
       <c r="V241" s="3"/>
     </row>
@@ -8873,10 +8872,10 @@
       <c r="L242" s="5"/>
       <c r="M242" s="8"/>
       <c r="O242" s="4"/>
-      <c r="P242" s="34"/>
-      <c r="Q242" s="34"/>
-      <c r="R242" s="34"/>
-      <c r="S242" s="35"/>
+      <c r="P242" s="33"/>
+      <c r="Q242" s="33"/>
+      <c r="R242" s="33"/>
+      <c r="S242" s="34"/>
       <c r="T242" s="1"/>
       <c r="V242" s="3"/>
     </row>
@@ -8894,10 +8893,10 @@
       <c r="L243" s="5"/>
       <c r="M243" s="8"/>
       <c r="O243" s="4"/>
-      <c r="P243" s="34"/>
-      <c r="Q243" s="34"/>
-      <c r="R243" s="34"/>
-      <c r="S243" s="35"/>
+      <c r="P243" s="33"/>
+      <c r="Q243" s="33"/>
+      <c r="R243" s="33"/>
+      <c r="S243" s="34"/>
       <c r="T243" s="1"/>
       <c r="V243" s="3"/>
     </row>
@@ -8915,10 +8914,10 @@
       <c r="L244" s="5"/>
       <c r="M244" s="8"/>
       <c r="O244" s="4"/>
-      <c r="P244" s="34"/>
-      <c r="Q244" s="34"/>
-      <c r="R244" s="34"/>
-      <c r="S244" s="35"/>
+      <c r="P244" s="33"/>
+      <c r="Q244" s="33"/>
+      <c r="R244" s="33"/>
+      <c r="S244" s="34"/>
       <c r="T244" s="1"/>
       <c r="V244" s="3"/>
     </row>
@@ -8936,10 +8935,10 @@
       <c r="L245" s="5"/>
       <c r="M245" s="8"/>
       <c r="O245" s="4"/>
-      <c r="P245" s="34"/>
-      <c r="Q245" s="34"/>
-      <c r="R245" s="34"/>
-      <c r="S245" s="35"/>
+      <c r="P245" s="33"/>
+      <c r="Q245" s="33"/>
+      <c r="R245" s="33"/>
+      <c r="S245" s="34"/>
       <c r="T245" s="1"/>
       <c r="V245" s="3"/>
     </row>
@@ -8957,10 +8956,10 @@
       <c r="L246" s="5"/>
       <c r="M246" s="8"/>
       <c r="O246" s="4"/>
-      <c r="P246" s="34"/>
-      <c r="Q246" s="34"/>
-      <c r="R246" s="34"/>
-      <c r="S246" s="35"/>
+      <c r="P246" s="33"/>
+      <c r="Q246" s="33"/>
+      <c r="R246" s="33"/>
+      <c r="S246" s="34"/>
       <c r="T246" s="1"/>
       <c r="V246" s="3"/>
     </row>
@@ -8978,10 +8977,10 @@
       <c r="L247" s="5"/>
       <c r="M247" s="8"/>
       <c r="O247" s="4"/>
-      <c r="P247" s="34"/>
-      <c r="Q247" s="34"/>
-      <c r="R247" s="34"/>
-      <c r="S247" s="35"/>
+      <c r="P247" s="33"/>
+      <c r="Q247" s="33"/>
+      <c r="R247" s="33"/>
+      <c r="S247" s="34"/>
       <c r="T247" s="1"/>
       <c r="V247" s="3"/>
     </row>
@@ -8999,10 +8998,10 @@
       <c r="L248" s="5"/>
       <c r="M248" s="8"/>
       <c r="O248" s="4"/>
-      <c r="P248" s="34"/>
-      <c r="Q248" s="34"/>
-      <c r="R248" s="34"/>
-      <c r="S248" s="35"/>
+      <c r="P248" s="33"/>
+      <c r="Q248" s="33"/>
+      <c r="R248" s="33"/>
+      <c r="S248" s="34"/>
       <c r="T248" s="1"/>
       <c r="V248" s="3"/>
     </row>
@@ -9020,10 +9019,10 @@
       <c r="L249" s="5"/>
       <c r="M249" s="8"/>
       <c r="O249" s="4"/>
-      <c r="P249" s="34"/>
-      <c r="Q249" s="34"/>
-      <c r="R249" s="34"/>
-      <c r="S249" s="35"/>
+      <c r="P249" s="33"/>
+      <c r="Q249" s="33"/>
+      <c r="R249" s="33"/>
+      <c r="S249" s="34"/>
       <c r="T249" s="1"/>
       <c r="V249" s="3"/>
     </row>
@@ -9041,10 +9040,10 @@
       <c r="L250" s="5"/>
       <c r="M250" s="8"/>
       <c r="O250" s="4"/>
-      <c r="P250" s="34"/>
-      <c r="Q250" s="34"/>
-      <c r="R250" s="34"/>
-      <c r="S250" s="35"/>
+      <c r="P250" s="33"/>
+      <c r="Q250" s="33"/>
+      <c r="R250" s="33"/>
+      <c r="S250" s="34"/>
       <c r="T250" s="1"/>
       <c r="V250" s="3"/>
     </row>
@@ -9062,10 +9061,10 @@
       <c r="L251" s="5"/>
       <c r="M251" s="8"/>
       <c r="O251" s="4"/>
-      <c r="P251" s="34"/>
-      <c r="Q251" s="34"/>
-      <c r="R251" s="34"/>
-      <c r="S251" s="35"/>
+      <c r="P251" s="33"/>
+      <c r="Q251" s="33"/>
+      <c r="R251" s="33"/>
+      <c r="S251" s="34"/>
       <c r="T251" s="1"/>
       <c r="V251" s="3"/>
     </row>
@@ -9083,10 +9082,10 @@
       <c r="L252" s="5"/>
       <c r="M252" s="8"/>
       <c r="O252" s="4"/>
-      <c r="P252" s="34"/>
-      <c r="Q252" s="34"/>
-      <c r="R252" s="34"/>
-      <c r="S252" s="35"/>
+      <c r="P252" s="33"/>
+      <c r="Q252" s="33"/>
+      <c r="R252" s="33"/>
+      <c r="S252" s="34"/>
       <c r="T252" s="1"/>
       <c r="V252" s="3"/>
     </row>
@@ -9104,10 +9103,10 @@
       <c r="L253" s="5"/>
       <c r="M253" s="8"/>
       <c r="O253" s="4"/>
-      <c r="P253" s="34"/>
-      <c r="Q253" s="34"/>
-      <c r="R253" s="34"/>
-      <c r="S253" s="35"/>
+      <c r="P253" s="33"/>
+      <c r="Q253" s="33"/>
+      <c r="R253" s="33"/>
+      <c r="S253" s="34"/>
       <c r="T253" s="1"/>
       <c r="V253" s="3"/>
     </row>
@@ -9125,10 +9124,10 @@
       <c r="L254" s="5"/>
       <c r="M254" s="8"/>
       <c r="O254" s="4"/>
-      <c r="P254" s="34"/>
-      <c r="Q254" s="34"/>
-      <c r="R254" s="34"/>
-      <c r="S254" s="35"/>
+      <c r="P254" s="33"/>
+      <c r="Q254" s="33"/>
+      <c r="R254" s="33"/>
+      <c r="S254" s="34"/>
       <c r="T254" s="1"/>
       <c r="V254" s="3"/>
     </row>
@@ -9146,10 +9145,10 @@
       <c r="L255" s="5"/>
       <c r="M255" s="8"/>
       <c r="O255" s="4"/>
-      <c r="P255" s="34"/>
-      <c r="Q255" s="34"/>
-      <c r="R255" s="34"/>
-      <c r="S255" s="35"/>
+      <c r="P255" s="33"/>
+      <c r="Q255" s="33"/>
+      <c r="R255" s="33"/>
+      <c r="S255" s="34"/>
       <c r="T255" s="1"/>
       <c r="V255" s="3"/>
     </row>
@@ -9167,10 +9166,10 @@
       <c r="L256" s="5"/>
       <c r="M256" s="8"/>
       <c r="O256" s="4"/>
-      <c r="P256" s="34"/>
-      <c r="Q256" s="34"/>
-      <c r="R256" s="34"/>
-      <c r="S256" s="35"/>
+      <c r="P256" s="33"/>
+      <c r="Q256" s="33"/>
+      <c r="R256" s="33"/>
+      <c r="S256" s="34"/>
       <c r="T256" s="1"/>
       <c r="V256" s="3"/>
     </row>
@@ -9188,10 +9187,10 @@
       <c r="L257" s="5"/>
       <c r="M257" s="8"/>
       <c r="O257" s="4"/>
-      <c r="P257" s="34"/>
-      <c r="Q257" s="34"/>
-      <c r="R257" s="34"/>
-      <c r="S257" s="35"/>
+      <c r="P257" s="33"/>
+      <c r="Q257" s="33"/>
+      <c r="R257" s="33"/>
+      <c r="S257" s="34"/>
       <c r="T257" s="1"/>
       <c r="V257" s="3"/>
     </row>
@@ -9209,10 +9208,10 @@
       <c r="L258" s="5"/>
       <c r="M258" s="8"/>
       <c r="O258" s="4"/>
-      <c r="P258" s="34"/>
-      <c r="Q258" s="34"/>
-      <c r="R258" s="34"/>
-      <c r="S258" s="35"/>
+      <c r="P258" s="33"/>
+      <c r="Q258" s="33"/>
+      <c r="R258" s="33"/>
+      <c r="S258" s="34"/>
       <c r="T258" s="1"/>
       <c r="V258" s="3"/>
     </row>
@@ -9230,10 +9229,10 @@
       <c r="L259" s="5"/>
       <c r="M259" s="8"/>
       <c r="O259" s="4"/>
-      <c r="P259" s="34"/>
-      <c r="Q259" s="34"/>
-      <c r="R259" s="34"/>
-      <c r="S259" s="35"/>
+      <c r="P259" s="33"/>
+      <c r="Q259" s="33"/>
+      <c r="R259" s="33"/>
+      <c r="S259" s="34"/>
       <c r="T259" s="1"/>
       <c r="V259" s="3"/>
     </row>
@@ -9251,10 +9250,10 @@
       <c r="L260" s="5"/>
       <c r="M260" s="8"/>
       <c r="O260" s="4"/>
-      <c r="P260" s="34"/>
-      <c r="Q260" s="34"/>
-      <c r="R260" s="34"/>
-      <c r="S260" s="35"/>
+      <c r="P260" s="33"/>
+      <c r="Q260" s="33"/>
+      <c r="R260" s="33"/>
+      <c r="S260" s="34"/>
       <c r="T260" s="1"/>
       <c r="V260" s="3"/>
     </row>
@@ -9272,10 +9271,10 @@
       <c r="L261" s="5"/>
       <c r="M261" s="8"/>
       <c r="O261" s="4"/>
-      <c r="P261" s="34"/>
-      <c r="Q261" s="34"/>
-      <c r="R261" s="34"/>
-      <c r="S261" s="35"/>
+      <c r="P261" s="33"/>
+      <c r="Q261" s="33"/>
+      <c r="R261" s="33"/>
+      <c r="S261" s="34"/>
       <c r="T261" s="1"/>
       <c r="V261" s="3"/>
     </row>
@@ -9293,10 +9292,10 @@
       <c r="L262" s="5"/>
       <c r="M262" s="8"/>
       <c r="O262" s="4"/>
-      <c r="P262" s="34"/>
-      <c r="Q262" s="34"/>
-      <c r="R262" s="34"/>
-      <c r="S262" s="35"/>
+      <c r="P262" s="33"/>
+      <c r="Q262" s="33"/>
+      <c r="R262" s="33"/>
+      <c r="S262" s="34"/>
       <c r="T262" s="1"/>
       <c r="V262" s="3"/>
     </row>
@@ -9314,10 +9313,10 @@
       <c r="L263" s="5"/>
       <c r="M263" s="8"/>
       <c r="O263" s="4"/>
-      <c r="P263" s="34"/>
-      <c r="Q263" s="34"/>
-      <c r="R263" s="34"/>
-      <c r="S263" s="35"/>
+      <c r="P263" s="33"/>
+      <c r="Q263" s="33"/>
+      <c r="R263" s="33"/>
+      <c r="S263" s="34"/>
       <c r="T263" s="1"/>
       <c r="V263" s="3"/>
     </row>
@@ -9335,10 +9334,10 @@
       <c r="L264" s="5"/>
       <c r="M264" s="8"/>
       <c r="O264" s="4"/>
-      <c r="P264" s="34"/>
-      <c r="Q264" s="34"/>
-      <c r="R264" s="34"/>
-      <c r="S264" s="35"/>
+      <c r="P264" s="33"/>
+      <c r="Q264" s="33"/>
+      <c r="R264" s="33"/>
+      <c r="S264" s="34"/>
       <c r="T264" s="1"/>
       <c r="V264" s="3"/>
     </row>
@@ -9356,10 +9355,10 @@
       <c r="L265" s="5"/>
       <c r="M265" s="8"/>
       <c r="O265" s="4"/>
-      <c r="P265" s="34"/>
-      <c r="Q265" s="34"/>
-      <c r="R265" s="34"/>
-      <c r="S265" s="35"/>
+      <c r="P265" s="33"/>
+      <c r="Q265" s="33"/>
+      <c r="R265" s="33"/>
+      <c r="S265" s="34"/>
       <c r="T265" s="1"/>
       <c r="V265" s="3"/>
     </row>
@@ -9377,10 +9376,10 @@
       <c r="L266" s="5"/>
       <c r="M266" s="8"/>
       <c r="O266" s="4"/>
-      <c r="P266" s="34"/>
-      <c r="Q266" s="34"/>
-      <c r="R266" s="34"/>
-      <c r="S266" s="35"/>
+      <c r="P266" s="33"/>
+      <c r="Q266" s="33"/>
+      <c r="R266" s="33"/>
+      <c r="S266" s="34"/>
       <c r="T266" s="1"/>
       <c r="V266" s="3"/>
     </row>
@@ -9398,10 +9397,10 @@
       <c r="L267" s="5"/>
       <c r="M267" s="8"/>
       <c r="O267" s="4"/>
-      <c r="P267" s="34"/>
-      <c r="Q267" s="34"/>
-      <c r="R267" s="34"/>
-      <c r="S267" s="35"/>
+      <c r="P267" s="33"/>
+      <c r="Q267" s="33"/>
+      <c r="R267" s="33"/>
+      <c r="S267" s="34"/>
       <c r="T267" s="1"/>
       <c r="V267" s="3"/>
     </row>
@@ -9419,10 +9418,10 @@
       <c r="L268" s="5"/>
       <c r="M268" s="8"/>
       <c r="O268" s="4"/>
-      <c r="P268" s="34"/>
-      <c r="Q268" s="34"/>
-      <c r="R268" s="34"/>
-      <c r="S268" s="35"/>
+      <c r="P268" s="33"/>
+      <c r="Q268" s="33"/>
+      <c r="R268" s="33"/>
+      <c r="S268" s="34"/>
       <c r="T268" s="1"/>
       <c r="V268" s="3"/>
     </row>
@@ -9440,10 +9439,10 @@
       <c r="L269" s="5"/>
       <c r="M269" s="8"/>
       <c r="O269" s="4"/>
-      <c r="P269" s="34"/>
-      <c r="Q269" s="34"/>
-      <c r="R269" s="34"/>
-      <c r="S269" s="35"/>
+      <c r="P269" s="33"/>
+      <c r="Q269" s="33"/>
+      <c r="R269" s="33"/>
+      <c r="S269" s="34"/>
       <c r="T269" s="1"/>
       <c r="V269" s="3"/>
     </row>
@@ -9461,10 +9460,10 @@
       <c r="L270" s="5"/>
       <c r="M270" s="8"/>
       <c r="O270" s="4"/>
-      <c r="P270" s="34"/>
-      <c r="Q270" s="34"/>
-      <c r="R270" s="34"/>
-      <c r="S270" s="35"/>
+      <c r="P270" s="33"/>
+      <c r="Q270" s="33"/>
+      <c r="R270" s="33"/>
+      <c r="S270" s="34"/>
       <c r="T270" s="1"/>
       <c r="V270" s="3"/>
     </row>
@@ -9482,10 +9481,10 @@
       <c r="L271" s="5"/>
       <c r="M271" s="8"/>
       <c r="O271" s="4"/>
-      <c r="P271" s="34"/>
-      <c r="Q271" s="34"/>
-      <c r="R271" s="34"/>
-      <c r="S271" s="35"/>
+      <c r="P271" s="33"/>
+      <c r="Q271" s="33"/>
+      <c r="R271" s="33"/>
+      <c r="S271" s="34"/>
       <c r="T271" s="1"/>
       <c r="V271" s="3"/>
     </row>
@@ -9503,10 +9502,10 @@
       <c r="L272" s="5"/>
       <c r="M272" s="8"/>
       <c r="O272" s="4"/>
-      <c r="P272" s="34"/>
-      <c r="Q272" s="34"/>
-      <c r="R272" s="34"/>
-      <c r="S272" s="35"/>
+      <c r="P272" s="33"/>
+      <c r="Q272" s="33"/>
+      <c r="R272" s="33"/>
+      <c r="S272" s="34"/>
       <c r="T272" s="1"/>
       <c r="V272" s="3"/>
     </row>
@@ -9524,10 +9523,10 @@
       <c r="L273" s="5"/>
       <c r="M273" s="8"/>
       <c r="O273" s="4"/>
-      <c r="P273" s="34"/>
-      <c r="Q273" s="34"/>
-      <c r="R273" s="34"/>
-      <c r="S273" s="35"/>
+      <c r="P273" s="33"/>
+      <c r="Q273" s="33"/>
+      <c r="R273" s="33"/>
+      <c r="S273" s="34"/>
       <c r="T273" s="1"/>
       <c r="V273" s="3"/>
     </row>
@@ -9545,10 +9544,10 @@
       <c r="L274" s="5"/>
       <c r="M274" s="8"/>
       <c r="O274" s="4"/>
-      <c r="P274" s="34"/>
-      <c r="Q274" s="34"/>
-      <c r="R274" s="34"/>
-      <c r="S274" s="35"/>
+      <c r="P274" s="33"/>
+      <c r="Q274" s="33"/>
+      <c r="R274" s="33"/>
+      <c r="S274" s="34"/>
       <c r="T274" s="1"/>
       <c r="V274" s="3"/>
     </row>
@@ -9566,10 +9565,10 @@
       <c r="L275" s="5"/>
       <c r="M275" s="8"/>
       <c r="O275" s="4"/>
-      <c r="P275" s="34"/>
-      <c r="Q275" s="34"/>
-      <c r="R275" s="34"/>
-      <c r="S275" s="35"/>
+      <c r="P275" s="33"/>
+      <c r="Q275" s="33"/>
+      <c r="R275" s="33"/>
+      <c r="S275" s="34"/>
       <c r="T275" s="1"/>
       <c r="V275" s="3"/>
     </row>
@@ -9586,7 +9585,7 @@
       <c r="K276" s="7"/>
       <c r="L276" s="5"/>
       <c r="M276" s="8"/>
-      <c r="O276" s="16"/>
+      <c r="O276" s="15"/>
       <c r="P276" s="37"/>
       <c r="Q276" s="37"/>
       <c r="R276" s="37"/>
@@ -9606,7 +9605,7 @@
       <c r="K277" s="7"/>
       <c r="L277" s="5"/>
       <c r="M277" s="8"/>
-      <c r="O277" s="16"/>
+      <c r="O277" s="15"/>
       <c r="P277" s="37"/>
       <c r="Q277" s="37"/>
       <c r="R277" s="37"/>
@@ -9626,7 +9625,7 @@
       <c r="K278" s="7"/>
       <c r="L278" s="5"/>
       <c r="M278" s="8"/>
-      <c r="O278" s="16"/>
+      <c r="O278" s="15"/>
       <c r="P278" s="37"/>
       <c r="Q278" s="37"/>
       <c r="R278" s="37"/>
@@ -9785,7 +9784,7 @@
       <c r="K288" s="13"/>
       <c r="L288" s="11"/>
       <c r="M288" s="14"/>
-      <c r="N288" s="15"/>
+      <c r="N288" s="35"/>
     </row>
     <row r="289" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C289" s="10"/>
@@ -9799,7 +9798,7 @@
       <c r="K289" s="13"/>
       <c r="L289" s="11"/>
       <c r="M289" s="14"/>
-      <c r="N289" s="15"/>
+      <c r="N289" s="35"/>
     </row>
     <row r="290" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C290" s="10"/>
@@ -9813,7 +9812,7 @@
       <c r="K290" s="13"/>
       <c r="L290" s="11"/>
       <c r="M290" s="14"/>
-      <c r="N290" s="15"/>
+      <c r="N290" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>